<commit_message>
Completamento dati mancanti LDO e correzione dati VPS su report_checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
+++ b/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\FSE_ACCREDITAMENTO\GATEWAY\S1#111PRAEZISIONX\PRAEZISION\ISOLABELLA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\FSE_ACCREDITAMENTO\GATEWAY\S1#111PRAEZISIONX\PRAEZISION\ISOLABELLA\3.29.0.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01F3B733-1561-434A-9512-513CE389B5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8AF9E-8D5E-409B-969F-2645AC1768F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2678" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="999">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -7731,10 +7731,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A129" sqref="A129"/>
-      <selection pane="topRight" activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="I9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="O215" sqref="O215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.33203125" defaultRowHeight="14.4"/>
@@ -7759,7 +7759,7 @@
     <col min="20" max="20" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" hidden="1">
       <c r="C1" s="4"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -7777,7 +7777,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="15"/>
     </row>
-    <row r="2" spans="1:20" ht="18">
+    <row r="2" spans="1:20" ht="18" hidden="1">
       <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
@@ -7800,7 +7800,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="15.6">
+    <row r="3" spans="1:20" ht="15.6" hidden="1">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
@@ -7825,7 +7825,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="15"/>
     </row>
-    <row r="4" spans="1:20" ht="15.6">
+    <row r="4" spans="1:20" ht="15.6" hidden="1">
       <c r="A4" s="42"/>
       <c r="B4" s="43"/>
       <c r="C4" s="46" t="s">
@@ -7849,7 +7849,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="15.6">
+    <row r="5" spans="1:20" ht="15.6" hidden="1">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="46" t="s">
@@ -7872,7 +7872,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" hidden="1">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
       <c r="C6" s="16"/>
@@ -7892,7 +7892,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" hidden="1">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -7912,7 +7912,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" hidden="1">
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -7991,7 +7991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="10" spans="1:20" ht="158.4" hidden="1">
       <c r="A10" s="20">
         <v>1</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="259.2" hidden="1">
+    <row r="11" spans="1:20" ht="158.4" hidden="1">
       <c r="A11" s="20">
         <v>2</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="144" hidden="1">
+    <row r="13" spans="1:20" ht="158.4" hidden="1">
       <c r="A13" s="20">
         <v>4</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="14" spans="1:20" ht="158.4" hidden="1">
       <c r="A14" s="20">
         <v>5</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="259.2">
+    <row r="15" spans="1:20" ht="144">
       <c r="A15" s="20">
         <v>6</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="288">
+    <row r="16" spans="1:20" ht="144">
       <c r="A16" s="20">
         <v>7</v>
       </c>
@@ -8253,7 +8253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="259.2">
+    <row r="17" spans="1:20" ht="144">
       <c r="A17" s="20">
         <v>8</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="288">
+    <row r="18" spans="1:20" ht="144">
       <c r="A18" s="20">
         <v>9</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="259.2" hidden="1">
+    <row r="19" spans="1:20" ht="144" hidden="1">
       <c r="A19" s="20">
         <v>11</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="22" spans="1:20" ht="144" hidden="1">
       <c r="A22" s="20">
         <v>14</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="259.2" hidden="1">
+    <row r="23" spans="1:20" ht="144" hidden="1">
       <c r="A23" s="20">
         <v>16</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="24" spans="1:20" ht="144" hidden="1">
       <c r="A24" s="20">
         <v>17</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="259.2" hidden="1">
+    <row r="25" spans="1:20" ht="144" hidden="1">
       <c r="A25" s="20">
         <v>18</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="216" hidden="1">
+    <row r="26" spans="1:20" ht="144" hidden="1">
       <c r="A26" s="20">
         <v>19</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="244.8" hidden="1">
+    <row r="27" spans="1:20" ht="144" hidden="1">
       <c r="A27" s="20">
         <v>20</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="158.4" hidden="1">
+    <row r="29" spans="1:20" ht="144" hidden="1">
       <c r="A29" s="20">
         <v>22</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="216" hidden="1">
+    <row r="30" spans="1:20" ht="144" hidden="1">
       <c r="A30" s="20">
         <v>23</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="244.8">
+    <row r="31" spans="1:20" ht="129.6">
       <c r="A31" s="20">
         <v>24</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="216">
+    <row r="32" spans="1:20" ht="129.6">
       <c r="A32" s="20">
         <v>25</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="244.8">
+    <row r="33" spans="1:20" ht="129.6">
       <c r="A33" s="20">
         <v>26</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="216">
+    <row r="34" spans="1:20" ht="129.6">
       <c r="A34" s="20">
         <v>27</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="244.8" hidden="1">
+    <row r="35" spans="1:20" ht="144" hidden="1">
       <c r="A35" s="20">
         <v>28</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="43.2">
+    <row r="36" spans="1:20" ht="144">
       <c r="A36" s="20">
         <v>29</v>
       </c>
@@ -9012,7 +9012,9 @@
       <c r="N36" s="25" t="s">
         <v>792</v>
       </c>
-      <c r="O36" s="25"/>
+      <c r="O36" s="25" t="s">
+        <v>788</v>
+      </c>
       <c r="P36" s="25" t="s">
         <v>791</v>
       </c>
@@ -9059,7 +9061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="216" hidden="1">
+    <row r="38" spans="1:20" ht="144" hidden="1">
       <c r="A38" s="20">
         <v>31</v>
       </c>
@@ -9093,7 +9095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="244.8" hidden="1">
+    <row r="39" spans="1:20" ht="144" hidden="1">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -9127,7 +9129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="216" hidden="1">
+    <row r="40" spans="1:20" ht="144" hidden="1">
       <c r="A40" s="20">
         <v>33</v>
       </c>
@@ -9161,7 +9163,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="244.8" hidden="1">
+    <row r="41" spans="1:20" ht="144" hidden="1">
       <c r="A41" s="20">
         <v>34</v>
       </c>
@@ -9251,7 +9253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="129.6" hidden="1">
+    <row r="43" spans="1:20" ht="158.4" hidden="1">
       <c r="A43" s="20">
         <v>36</v>
       </c>
@@ -9326,7 +9328,9 @@
       <c r="N44" s="25" t="s">
         <v>792</v>
       </c>
-      <c r="O44" s="25"/>
+      <c r="O44" s="25" t="s">
+        <v>788</v>
+      </c>
       <c r="P44" s="25" t="s">
         <v>791</v>
       </c>
@@ -9339,7 +9343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="115.2" hidden="1">
+    <row r="45" spans="1:20" ht="158.4" hidden="1">
       <c r="A45" s="20">
         <v>38</v>
       </c>
@@ -9407,7 +9411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="129.6" hidden="1">
+    <row r="47" spans="1:20" ht="158.4" hidden="1">
       <c r="A47" s="20">
         <v>40</v>
       </c>
@@ -9441,7 +9445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="172.8" hidden="1">
+    <row r="48" spans="1:20" ht="158.4" hidden="1">
       <c r="A48" s="20">
         <v>41</v>
       </c>
@@ -9475,7 +9479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="129.6" hidden="1">
+    <row r="49" spans="1:20" ht="158.4" hidden="1">
       <c r="A49" s="20">
         <v>42</v>
       </c>
@@ -9565,7 +9569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="129.6" hidden="1">
+    <row r="51" spans="1:20" ht="43.2" hidden="1">
       <c r="A51" s="20">
         <v>44</v>
       </c>
@@ -9601,7 +9605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="129.6">
+    <row r="52" spans="1:20" ht="43.2">
       <c r="A52" s="20">
         <v>45</v>
       </c>
@@ -9634,7 +9638,9 @@
       <c r="N52" s="25" t="s">
         <v>793</v>
       </c>
-      <c r="O52" s="25"/>
+      <c r="O52" s="25" t="s">
+        <v>788</v>
+      </c>
       <c r="P52" s="25" t="s">
         <v>796</v>
       </c>
@@ -9649,7 +9655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="144" hidden="1">
+    <row r="53" spans="1:20" ht="43.2" hidden="1">
       <c r="A53" s="20">
         <v>46</v>
       </c>
@@ -9685,7 +9691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="158.4" hidden="1">
+    <row r="54" spans="1:20" ht="43.2" hidden="1">
       <c r="A54" s="20">
         <v>47</v>
       </c>
@@ -9721,7 +9727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="129.6" hidden="1">
+    <row r="55" spans="1:20" ht="43.2" hidden="1">
       <c r="A55" s="20">
         <v>48</v>
       </c>
@@ -9757,7 +9763,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="158.4" hidden="1">
+    <row r="56" spans="1:20" ht="43.2" hidden="1">
       <c r="A56" s="20">
         <v>49</v>
       </c>
@@ -9793,7 +9799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="129.6" hidden="1">
+    <row r="57" spans="1:20" ht="43.2" hidden="1">
       <c r="A57" s="20">
         <v>50</v>
       </c>
@@ -9829,7 +9835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="288">
+    <row r="58" spans="1:20" ht="129.6">
       <c r="A58" s="20">
         <v>51</v>
       </c>
@@ -9862,7 +9868,9 @@
       <c r="N58" s="25" t="s">
         <v>793</v>
       </c>
-      <c r="O58" s="25"/>
+      <c r="O58" s="25" t="s">
+        <v>788</v>
+      </c>
       <c r="P58" s="25" t="s">
         <v>796</v>
       </c>
@@ -9877,7 +9885,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="259.2" hidden="1">
+    <row r="59" spans="1:20" ht="115.2" hidden="1">
       <c r="A59" s="20">
         <v>52</v>
       </c>
@@ -9911,7 +9919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="144" hidden="1">
+    <row r="60" spans="1:20" ht="115.2" hidden="1">
       <c r="A60" s="20">
         <v>53</v>
       </c>
@@ -9979,7 +9987,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="288" hidden="1">
+    <row r="62" spans="1:20" ht="115.2" hidden="1">
       <c r="A62" s="20">
         <v>55</v>
       </c>
@@ -10013,7 +10021,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="259.2" hidden="1">
+    <row r="63" spans="1:20" ht="115.2" hidden="1">
       <c r="A63" s="20">
         <v>56</v>
       </c>
@@ -10047,7 +10055,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="64" spans="1:20" ht="115.2" hidden="1">
       <c r="A64" s="20">
         <v>57</v>
       </c>
@@ -10081,7 +10089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="259.2" hidden="1">
+    <row r="65" spans="1:20" ht="115.2" hidden="1">
       <c r="A65" s="20">
         <v>58</v>
       </c>
@@ -10115,7 +10123,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="66" spans="1:20" ht="115.2" hidden="1">
       <c r="A66" s="20">
         <v>59</v>
       </c>
@@ -10149,7 +10157,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="259.2" hidden="1">
+    <row r="67" spans="1:20" ht="115.2" hidden="1">
       <c r="A67" s="20">
         <v>60</v>
       </c>
@@ -10183,7 +10191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="129.6" hidden="1">
+    <row r="68" spans="1:20" ht="115.2" hidden="1">
       <c r="A68" s="20">
         <v>61</v>
       </c>
@@ -10217,7 +10225,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="144" hidden="1">
+    <row r="69" spans="1:20" ht="115.2" hidden="1">
       <c r="A69" s="20">
         <v>62</v>
       </c>
@@ -10251,7 +10259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="288">
+    <row r="70" spans="1:20" ht="129.6">
       <c r="A70" s="20">
         <v>63</v>
       </c>
@@ -10292,7 +10300,9 @@
       <c r="N70" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O70" s="25"/>
+      <c r="O70" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P70" s="25" t="s">
         <v>795</v>
       </c>
@@ -10305,7 +10315,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="259.2">
+    <row r="71" spans="1:20" ht="129.6">
       <c r="A71" s="20">
         <v>64</v>
       </c>
@@ -10346,7 +10356,9 @@
       <c r="N71" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O71" s="25"/>
+      <c r="O71" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P71" s="25" t="s">
         <v>795</v>
       </c>
@@ -10359,7 +10371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="288">
+    <row r="72" spans="1:20" ht="129.6">
       <c r="A72" s="20">
         <v>65</v>
       </c>
@@ -10400,7 +10412,9 @@
       <c r="N72" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O72" s="25"/>
+      <c r="O72" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P72" s="25" t="s">
         <v>795</v>
       </c>
@@ -10413,7 +10427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="259.2">
+    <row r="73" spans="1:20" ht="129.6">
       <c r="A73" s="20">
         <v>66</v>
       </c>
@@ -10454,7 +10468,9 @@
       <c r="N73" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O73" s="25"/>
+      <c r="O73" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P73" s="25" t="s">
         <v>795</v>
       </c>
@@ -10467,7 +10483,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="216">
+    <row r="74" spans="1:20" ht="129.6">
       <c r="A74" s="20">
         <v>67</v>
       </c>
@@ -10508,7 +10524,9 @@
       <c r="N74" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O74" s="25"/>
+      <c r="O74" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P74" s="25" t="s">
         <v>795</v>
       </c>
@@ -10521,7 +10539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="201.6">
+    <row r="75" spans="1:20" ht="129.6">
       <c r="A75" s="20">
         <v>68</v>
       </c>
@@ -10562,7 +10580,9 @@
       <c r="N75" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O75" s="25"/>
+      <c r="O75" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P75" s="25" t="s">
         <v>795</v>
       </c>
@@ -10575,7 +10595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="230.4">
+    <row r="76" spans="1:20" ht="129.6">
       <c r="A76" s="20">
         <v>69</v>
       </c>
@@ -10616,7 +10636,9 @@
       <c r="N76" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O76" s="25"/>
+      <c r="O76" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P76" s="25" t="s">
         <v>795</v>
       </c>
@@ -10629,7 +10651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="244.8">
+    <row r="77" spans="1:20" ht="129.6">
       <c r="A77" s="20">
         <v>70</v>
       </c>
@@ -10670,7 +10692,9 @@
       <c r="N77" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O77" s="25"/>
+      <c r="O77" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P77" s="25" t="s">
         <v>795</v>
       </c>
@@ -10683,7 +10707,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="244.8">
+    <row r="78" spans="1:20" ht="129.6">
       <c r="A78" s="20">
         <v>71</v>
       </c>
@@ -10724,7 +10748,9 @@
       <c r="N78" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O78" s="25"/>
+      <c r="O78" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P78" s="25" t="s">
         <v>795</v>
       </c>
@@ -10737,7 +10763,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="244.8">
+    <row r="79" spans="1:20" ht="129.6">
       <c r="A79" s="20">
         <v>72</v>
       </c>
@@ -10778,7 +10804,9 @@
       <c r="N79" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O79" s="25"/>
+      <c r="O79" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P79" s="25" t="s">
         <v>795</v>
       </c>
@@ -10791,7 +10819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="244.8">
+    <row r="80" spans="1:20" ht="129.6">
       <c r="A80" s="20">
         <v>73</v>
       </c>
@@ -10832,7 +10860,9 @@
       <c r="N80" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O80" s="25"/>
+      <c r="O80" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P80" s="25" t="s">
         <v>795</v>
       </c>
@@ -10845,7 +10875,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="244.8">
+    <row r="81" spans="1:20" ht="129.6">
       <c r="A81" s="20">
         <v>74</v>
       </c>
@@ -10886,7 +10916,9 @@
       <c r="N81" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="O81" s="25"/>
+      <c r="O81" s="25" t="s">
+        <v>483</v>
+      </c>
       <c r="P81" s="25" t="s">
         <v>795</v>
       </c>
@@ -10933,7 +10965,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="115.2" hidden="1">
+    <row r="83" spans="1:20" ht="129.6" hidden="1">
       <c r="A83" s="20">
         <v>76</v>
       </c>
@@ -10967,7 +10999,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="144" hidden="1">
+    <row r="84" spans="1:20" ht="115.2" hidden="1">
       <c r="A84" s="20">
         <v>77</v>
       </c>
@@ -11001,7 +11033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="216" hidden="1">
+    <row r="85" spans="1:20" ht="115.2" hidden="1">
       <c r="A85" s="20">
         <v>78</v>
       </c>
@@ -11035,7 +11067,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="288" hidden="1">
+    <row r="86" spans="1:20" ht="129.6" hidden="1">
       <c r="A86" s="20">
         <v>79</v>
       </c>
@@ -11069,7 +11101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="87" spans="1:20" ht="129.6" hidden="1">
       <c r="A87" s="20">
         <v>80</v>
       </c>
@@ -11103,7 +11135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="158.4" hidden="1">
+    <row r="88" spans="1:20" ht="129.6" hidden="1">
       <c r="A88" s="20">
         <v>81</v>
       </c>
@@ -11137,7 +11169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="288" hidden="1">
+    <row r="89" spans="1:20" ht="129.6" hidden="1">
       <c r="A89" s="20">
         <v>82</v>
       </c>
@@ -11171,7 +11203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="216" hidden="1">
+    <row r="90" spans="1:20" ht="115.2" hidden="1">
       <c r="A90" s="20">
         <v>83</v>
       </c>
@@ -11205,7 +11237,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="201.6" hidden="1">
+    <row r="91" spans="1:20" ht="115.2" hidden="1">
       <c r="A91" s="20">
         <v>84</v>
       </c>
@@ -11239,7 +11271,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="230.4" hidden="1">
+    <row r="92" spans="1:20" ht="129.6" hidden="1">
       <c r="A92" s="20">
         <v>85</v>
       </c>
@@ -11273,7 +11305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="244.8" hidden="1">
+    <row r="93" spans="1:20" ht="129.6" hidden="1">
       <c r="A93" s="20">
         <v>86</v>
       </c>
@@ -11307,7 +11339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="244.8" hidden="1">
+    <row r="94" spans="1:20" ht="144" hidden="1">
       <c r="A94" s="20">
         <v>87</v>
       </c>
@@ -11341,7 +11373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="244.8" hidden="1">
+    <row r="95" spans="1:20" ht="129.6" hidden="1">
       <c r="A95" s="20">
         <v>88</v>
       </c>
@@ -11375,7 +11407,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="244.8" hidden="1">
+    <row r="96" spans="1:20" ht="115.2" hidden="1">
       <c r="A96" s="20">
         <v>89</v>
       </c>
@@ -11409,7 +11441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="244.8" hidden="1">
+    <row r="97" spans="1:20" ht="115.2" hidden="1">
       <c r="A97" s="20">
         <v>90</v>
       </c>
@@ -11443,7 +11475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="216" hidden="1">
+    <row r="98" spans="1:20" ht="129.6" hidden="1">
       <c r="A98" s="20">
         <v>91</v>
       </c>
@@ -11477,7 +11509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="201.6" hidden="1">
+    <row r="99" spans="1:20" ht="129.6" hidden="1">
       <c r="A99" s="20">
         <v>92</v>
       </c>
@@ -11511,7 +11543,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="230.4" hidden="1">
+    <row r="100" spans="1:20" ht="129.6" hidden="1">
       <c r="A100" s="20">
         <v>93</v>
       </c>
@@ -11545,7 +11577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="244.8" hidden="1">
+    <row r="101" spans="1:20" ht="144" hidden="1">
       <c r="A101" s="20">
         <v>94</v>
       </c>
@@ -11579,7 +11611,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="244.8" hidden="1">
+    <row r="102" spans="1:20" ht="144" hidden="1">
       <c r="A102" s="20">
         <v>95</v>
       </c>
@@ -11613,7 +11645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="244.8" hidden="1">
+    <row r="103" spans="1:20" ht="115.2" hidden="1">
       <c r="A103" s="20">
         <v>96</v>
       </c>
@@ -11647,7 +11679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="244.8" hidden="1">
+    <row r="104" spans="1:20" ht="129.6" hidden="1">
       <c r="A104" s="20">
         <v>97</v>
       </c>
@@ -11681,7 +11713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="244.8" hidden="1">
+    <row r="105" spans="1:20" ht="144" hidden="1">
       <c r="A105" s="20">
         <v>98</v>
       </c>
@@ -11715,7 +11747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="216" hidden="1">
+    <row r="106" spans="1:20" ht="144" hidden="1">
       <c r="A106" s="20">
         <v>99</v>
       </c>
@@ -11749,7 +11781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="201.6" hidden="1">
+    <row r="107" spans="1:20" ht="115.2" hidden="1">
       <c r="A107" s="20">
         <v>100</v>
       </c>
@@ -11783,7 +11815,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="230.4" hidden="1">
+    <row r="108" spans="1:20" ht="129.6" hidden="1">
       <c r="A108" s="20">
         <v>101</v>
       </c>
@@ -11817,7 +11849,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="244.8" hidden="1">
+    <row r="109" spans="1:20" ht="144" hidden="1">
       <c r="A109" s="20">
         <v>102</v>
       </c>
@@ -11851,7 +11883,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="244.8" hidden="1">
+    <row r="110" spans="1:20" ht="144" hidden="1">
       <c r="A110" s="20">
         <v>103</v>
       </c>
@@ -11885,7 +11917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="244.8" hidden="1">
+    <row r="111" spans="1:20" ht="115.2" hidden="1">
       <c r="A111" s="20">
         <v>104</v>
       </c>
@@ -11919,7 +11951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="244.8" hidden="1">
+    <row r="112" spans="1:20" ht="144" hidden="1">
       <c r="A112" s="20">
         <v>105</v>
       </c>
@@ -11953,7 +11985,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="244.8" hidden="1">
+    <row r="113" spans="1:20" ht="144" hidden="1">
       <c r="A113" s="20">
         <v>106</v>
       </c>
@@ -11987,7 +12019,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="201.6" hidden="1">
+    <row r="114" spans="1:20" ht="129.6" hidden="1">
       <c r="A114" s="20">
         <v>107</v>
       </c>
@@ -12021,7 +12053,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="230.4" hidden="1">
+    <row r="115" spans="1:20" ht="129.6" hidden="1">
       <c r="A115" s="20">
         <v>108</v>
       </c>
@@ -12055,7 +12087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="244.8" hidden="1">
+    <row r="116" spans="1:20" ht="129.6" hidden="1">
       <c r="A116" s="20">
         <v>109</v>
       </c>
@@ -12089,7 +12121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="244.8" hidden="1">
+    <row r="117" spans="1:20" ht="115.2" hidden="1">
       <c r="A117" s="20">
         <v>110</v>
       </c>
@@ -12123,7 +12155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="244.8" hidden="1">
+    <row r="118" spans="1:20" ht="129.6" hidden="1">
       <c r="A118" s="20">
         <v>111</v>
       </c>
@@ -12157,7 +12189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="244.8" hidden="1">
+    <row r="119" spans="1:20" ht="129.6" hidden="1">
       <c r="A119" s="20">
         <v>112</v>
       </c>
@@ -12191,7 +12223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="244.8" hidden="1">
+    <row r="120" spans="1:20" ht="129.6" hidden="1">
       <c r="A120" s="20">
         <v>113</v>
       </c>
@@ -12259,7 +12291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="216" hidden="1">
+    <row r="122" spans="1:20" ht="129.6" hidden="1">
       <c r="A122" s="20">
         <v>115</v>
       </c>
@@ -12293,7 +12325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="201.6" hidden="1">
+    <row r="123" spans="1:20" ht="129.6" hidden="1">
       <c r="A123" s="20">
         <v>116</v>
       </c>
@@ -12327,7 +12359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="230.4" hidden="1">
+    <row r="124" spans="1:20" ht="129.6" hidden="1">
       <c r="A124" s="20">
         <v>117</v>
       </c>
@@ -12361,7 +12393,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="244.8" hidden="1">
+    <row r="125" spans="1:20" ht="129.6" hidden="1">
       <c r="A125" s="20">
         <v>118</v>
       </c>
@@ -12395,7 +12427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="244.8" hidden="1">
+    <row r="126" spans="1:20" ht="129.6" hidden="1">
       <c r="A126" s="20">
         <v>119</v>
       </c>
@@ -12429,7 +12461,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="244.8" hidden="1">
+    <row r="127" spans="1:20" ht="129.6" hidden="1">
       <c r="A127" s="20">
         <v>120</v>
       </c>
@@ -12463,7 +12495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="244.8" hidden="1">
+    <row r="128" spans="1:20" ht="129.6" hidden="1">
       <c r="A128" s="20">
         <v>121</v>
       </c>
@@ -12539,7 +12571,7 @@
         <v>794</v>
       </c>
       <c r="O129" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P129" s="25" t="s">
         <v>795</v>
@@ -12595,7 +12627,7 @@
         <v>794</v>
       </c>
       <c r="O130" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P130" s="25" t="s">
         <v>795</v>
@@ -12651,7 +12683,7 @@
         <v>794</v>
       </c>
       <c r="O131" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P131" s="25" t="s">
         <v>795</v>
@@ -12707,7 +12739,7 @@
         <v>794</v>
       </c>
       <c r="O132" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P132" s="25" t="s">
         <v>795</v>
@@ -12763,7 +12795,7 @@
         <v>794</v>
       </c>
       <c r="O133" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P133" s="25" t="s">
         <v>795</v>
@@ -12819,7 +12851,7 @@
         <v>794</v>
       </c>
       <c r="O134" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P134" s="25" t="s">
         <v>795</v>
@@ -12875,7 +12907,7 @@
         <v>794</v>
       </c>
       <c r="O135" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P135" s="25" t="s">
         <v>795</v>
@@ -12931,7 +12963,7 @@
         <v>794</v>
       </c>
       <c r="O136" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P136" s="25" t="s">
         <v>795</v>
@@ -12987,7 +13019,7 @@
         <v>794</v>
       </c>
       <c r="O137" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P137" s="25" t="s">
         <v>795</v>
@@ -13043,7 +13075,7 @@
         <v>794</v>
       </c>
       <c r="O138" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P138" s="25" t="s">
         <v>795</v>
@@ -13099,7 +13131,7 @@
         <v>794</v>
       </c>
       <c r="O139" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P139" s="25" t="s">
         <v>795</v>
@@ -13155,7 +13187,7 @@
         <v>794</v>
       </c>
       <c r="O140" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P140" s="25" t="s">
         <v>795</v>
@@ -13211,7 +13243,7 @@
         <v>794</v>
       </c>
       <c r="O141" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P141" s="25" t="s">
         <v>795</v>
@@ -13267,7 +13299,7 @@
         <v>794</v>
       </c>
       <c r="O142" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P142" s="25" t="s">
         <v>795</v>
@@ -13323,7 +13355,7 @@
         <v>794</v>
       </c>
       <c r="O143" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P143" s="25" t="s">
         <v>795</v>
@@ -13379,7 +13411,7 @@
         <v>794</v>
       </c>
       <c r="O144" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P144" s="25" t="s">
         <v>795</v>
@@ -13435,7 +13467,7 @@
         <v>794</v>
       </c>
       <c r="O145" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P145" s="25" t="s">
         <v>795</v>
@@ -13491,7 +13523,7 @@
         <v>794</v>
       </c>
       <c r="O146" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P146" s="25" t="s">
         <v>795</v>
@@ -13547,7 +13579,7 @@
         <v>794</v>
       </c>
       <c r="O147" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P147" s="25" t="s">
         <v>795</v>
@@ -13603,7 +13635,7 @@
         <v>794</v>
       </c>
       <c r="O148" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P148" s="25" t="s">
         <v>795</v>
@@ -13659,7 +13691,7 @@
         <v>794</v>
       </c>
       <c r="O149" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P149" s="25" t="s">
         <v>795</v>
@@ -13715,7 +13747,7 @@
         <v>794</v>
       </c>
       <c r="O150" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P150" s="25" t="s">
         <v>795</v>
@@ -13771,7 +13803,7 @@
         <v>794</v>
       </c>
       <c r="O151" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P151" s="25" t="s">
         <v>795</v>
@@ -13827,7 +13859,7 @@
         <v>794</v>
       </c>
       <c r="O152" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P152" s="25" t="s">
         <v>795</v>
@@ -13883,7 +13915,7 @@
         <v>794</v>
       </c>
       <c r="O153" s="25" t="s">
-        <v>788</v>
+        <v>483</v>
       </c>
       <c r="P153" s="25" t="s">
         <v>795</v>
@@ -13897,7 +13929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="288" hidden="1">
+    <row r="154" spans="1:20" ht="158.4" hidden="1">
       <c r="A154" s="20">
         <v>147</v>
       </c>
@@ -13931,7 +13963,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="155" spans="1:20" ht="158.4" hidden="1">
       <c r="A155" s="20">
         <v>148</v>
       </c>
@@ -13965,7 +13997,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="259.2" hidden="1">
+    <row r="156" spans="1:20" ht="158.4" hidden="1">
       <c r="A156" s="20">
         <v>149</v>
       </c>
@@ -13999,7 +14031,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="244.8" hidden="1">
+    <row r="157" spans="1:20" ht="158.4" hidden="1">
       <c r="A157" s="20">
         <v>150</v>
       </c>
@@ -14033,7 +14065,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="288" hidden="1">
+    <row r="158" spans="1:20" ht="115.2" hidden="1">
       <c r="A158" s="20">
         <v>151</v>
       </c>
@@ -14067,7 +14099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="288" hidden="1">
+    <row r="159" spans="1:20" ht="129.6" hidden="1">
       <c r="A159" s="20">
         <v>152</v>
       </c>
@@ -14101,7 +14133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="160" spans="1:20" ht="129.6" hidden="1">
       <c r="A160" s="20">
         <v>153</v>
       </c>
@@ -14135,7 +14167,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="288" hidden="1">
+    <row r="161" spans="1:20" ht="129.6" hidden="1">
       <c r="A161" s="20">
         <v>154</v>
       </c>
@@ -14169,7 +14201,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="162" spans="1:20" ht="129.6" hidden="1">
       <c r="A162" s="20">
         <v>155</v>
       </c>
@@ -14203,7 +14235,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="288" hidden="1">
+    <row r="163" spans="1:20" ht="129.6" hidden="1">
       <c r="A163" s="20">
         <v>156</v>
       </c>
@@ -14237,7 +14269,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="164" spans="1:20" ht="129.6" hidden="1">
       <c r="A164" s="20">
         <v>157</v>
       </c>
@@ -14271,7 +14303,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="216" hidden="1">
+    <row r="165" spans="1:20" ht="129.6" hidden="1">
       <c r="A165" s="20">
         <v>158</v>
       </c>
@@ -14305,7 +14337,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="288" hidden="1">
+    <row r="166" spans="1:20" ht="115.2" hidden="1">
       <c r="A166" s="20">
         <v>159</v>
       </c>
@@ -14339,7 +14371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="288" hidden="1">
+    <row r="167" spans="1:20" ht="115.2" hidden="1">
       <c r="A167" s="20">
         <v>160</v>
       </c>
@@ -14373,7 +14405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="288" hidden="1">
+    <row r="168" spans="1:20" ht="129.6" hidden="1">
       <c r="A168" s="20">
         <v>161</v>
       </c>
@@ -14407,7 +14439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="288" hidden="1">
+    <row r="169" spans="1:20" ht="129.6" hidden="1">
       <c r="A169" s="20">
         <v>162</v>
       </c>
@@ -14441,7 +14473,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="244.8" hidden="1">
+    <row r="170" spans="1:20" ht="129.6" hidden="1">
       <c r="A170" s="20">
         <v>163</v>
       </c>
@@ -14475,7 +14507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="171" spans="1:20" ht="129.6" hidden="1">
       <c r="A171" s="20">
         <v>164</v>
       </c>
@@ -14509,7 +14541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="244.8" hidden="1">
+    <row r="172" spans="1:20" ht="129.6" hidden="1">
       <c r="A172" s="20">
         <v>165</v>
       </c>
@@ -14543,7 +14575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="144" hidden="1">
+    <row r="173" spans="1:20" ht="129.6" hidden="1">
       <c r="A173" s="20">
         <v>166</v>
       </c>
@@ -14577,7 +14609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="244.8" hidden="1">
+    <row r="174" spans="1:20" ht="129.6" hidden="1">
       <c r="A174" s="20">
         <v>167</v>
       </c>
@@ -14611,7 +14643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="175" spans="1:20" ht="129.6" hidden="1">
       <c r="A175" s="20">
         <v>168</v>
       </c>
@@ -14645,7 +14677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="230.4" hidden="1">
+    <row r="176" spans="1:20" ht="129.6" hidden="1">
       <c r="A176" s="20">
         <v>169</v>
       </c>
@@ -14679,7 +14711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="177" spans="1:20" ht="158.4" hidden="1">
       <c r="A177" s="20">
         <v>170</v>
       </c>
@@ -14713,7 +14745,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="244.8" hidden="1">
+    <row r="178" spans="1:20" ht="158.4" hidden="1">
       <c r="A178" s="20">
         <v>171</v>
       </c>
@@ -14747,7 +14779,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="179" spans="1:20" ht="158.4" hidden="1">
       <c r="A179" s="20">
         <v>172</v>
       </c>
@@ -14815,7 +14847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="158.4" hidden="1">
+    <row r="181" spans="1:20" ht="115.2" hidden="1">
       <c r="A181" s="20">
         <v>174</v>
       </c>
@@ -14849,7 +14881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="230.4" hidden="1">
+    <row r="182" spans="1:20" ht="129.6" hidden="1">
       <c r="A182" s="20">
         <v>175</v>
       </c>
@@ -14883,7 +14915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="183" spans="1:20" ht="129.6" hidden="1">
       <c r="A183" s="20">
         <v>176</v>
       </c>
@@ -14917,7 +14949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="244.8" hidden="1">
+    <row r="184" spans="1:20" ht="129.6" hidden="1">
       <c r="A184" s="20">
         <v>177</v>
       </c>
@@ -14951,7 +14983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="185" spans="1:20" ht="129.6" hidden="1">
       <c r="A185" s="20">
         <v>178</v>
       </c>
@@ -14985,7 +15017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="158.4" hidden="1">
+    <row r="186" spans="1:20" ht="129.6" hidden="1">
       <c r="A186" s="20">
         <v>179</v>
       </c>
@@ -15019,7 +15051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="158.4" hidden="1">
+    <row r="187" spans="1:20" ht="129.6" hidden="1">
       <c r="A187" s="20">
         <v>180</v>
       </c>
@@ -15053,7 +15085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="158.4" hidden="1">
+    <row r="188" spans="1:20" ht="115.2" hidden="1">
       <c r="A188" s="20">
         <v>181</v>
       </c>
@@ -15087,7 +15119,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="144" hidden="1">
+    <row r="189" spans="1:20" ht="129.6" hidden="1">
       <c r="A189" s="20">
         <v>182</v>
       </c>
@@ -15121,7 +15153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="158.4" hidden="1">
+    <row r="190" spans="1:20" ht="129.6" hidden="1">
       <c r="A190" s="20">
         <v>183</v>
       </c>
@@ -15155,7 +15187,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="43.2" hidden="1">
+    <row r="191" spans="1:20" ht="129.6" hidden="1">
       <c r="A191" s="20">
         <v>184</v>
       </c>
@@ -15189,7 +15221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="115.2" hidden="1">
+    <row r="192" spans="1:20" ht="129.6" hidden="1">
       <c r="A192" s="20">
         <v>185</v>
       </c>
@@ -15223,7 +15255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="115.2" hidden="1">
+    <row r="193" spans="1:20" ht="129.6" hidden="1">
       <c r="A193" s="20">
         <v>186</v>
       </c>
@@ -15257,7 +15289,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="115.2" hidden="1">
+    <row r="194" spans="1:20" ht="129.6" hidden="1">
       <c r="A194" s="20">
         <v>187</v>
       </c>
@@ -15291,7 +15323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="115.2" hidden="1">
+    <row r="195" spans="1:20" ht="129.6" hidden="1">
       <c r="A195" s="20">
         <v>188</v>
       </c>
@@ -15325,7 +15357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="115.2" hidden="1">
+    <row r="196" spans="1:20" ht="129.6" hidden="1">
       <c r="A196" s="20">
         <v>189</v>
       </c>
@@ -15359,7 +15391,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="115.2" hidden="1">
+    <row r="197" spans="1:20" ht="129.6" hidden="1">
       <c r="A197" s="20">
         <v>190</v>
       </c>
@@ -15393,7 +15425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="115.2" hidden="1">
+    <row r="198" spans="1:20" ht="158.4" hidden="1">
       <c r="A198" s="20">
         <v>191</v>
       </c>
@@ -15427,7 +15459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="115.2" hidden="1">
+    <row r="199" spans="1:20" ht="216" hidden="1">
       <c r="A199" s="20">
         <v>192</v>
       </c>
@@ -15461,7 +15493,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="115.2" hidden="1">
+    <row r="200" spans="1:20" ht="288" hidden="1">
       <c r="A200" s="20">
         <v>193</v>
       </c>
@@ -15495,7 +15527,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="115.2" hidden="1">
+    <row r="201" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A201" s="20">
         <v>194</v>
       </c>
@@ -15529,7 +15561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="115.2" hidden="1">
+    <row r="202" spans="1:20" ht="158.4" hidden="1">
       <c r="A202" s="20">
         <v>195</v>
       </c>
@@ -15563,7 +15595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="158.4" hidden="1">
+    <row r="203" spans="1:20" ht="288" hidden="1">
       <c r="A203" s="20">
         <v>196</v>
       </c>
@@ -15597,7 +15629,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="144" hidden="1">
+    <row r="204" spans="1:20" ht="201.6" hidden="1">
       <c r="A204" s="20">
         <v>197</v>
       </c>
@@ -15631,7 +15663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="144" hidden="1">
+    <row r="205" spans="1:20" ht="230.4" hidden="1">
       <c r="A205" s="20">
         <v>198</v>
       </c>
@@ -15665,7 +15697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="144" hidden="1">
+    <row r="206" spans="1:20" ht="244.8" hidden="1">
       <c r="A206" s="20">
         <v>199</v>
       </c>
@@ -15699,7 +15731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="144" hidden="1">
+    <row r="207" spans="1:20" ht="244.8" hidden="1">
       <c r="A207" s="20">
         <v>200</v>
       </c>
@@ -15733,7 +15765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="144" hidden="1">
+    <row r="208" spans="1:20" ht="244.8" hidden="1">
       <c r="A208" s="20">
         <v>201</v>
       </c>
@@ -15767,7 +15799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="158.4" hidden="1">
+    <row r="209" spans="1:20" ht="244.8" hidden="1">
       <c r="A209" s="20">
         <v>202</v>
       </c>
@@ -15801,7 +15833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="43.2" hidden="1">
+    <row r="210" spans="1:20" ht="244.8" hidden="1">
       <c r="A210" s="20">
         <v>203</v>
       </c>
@@ -15869,7 +15901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="129.6" hidden="1">
+    <row r="212" spans="1:20" ht="259.2" hidden="1">
       <c r="A212" s="20">
         <v>205</v>
       </c>
@@ -15903,7 +15935,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="129.6" hidden="1">
+    <row r="213" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A213" s="20">
         <v>206</v>
       </c>
@@ -15937,7 +15969,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="129.6" hidden="1">
+    <row r="214" spans="1:20" ht="259.2" hidden="1">
       <c r="A214" s="20">
         <v>207</v>
       </c>
@@ -15971,7 +16003,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="129.6">
+    <row r="215" spans="1:20" ht="216">
       <c r="A215" s="20">
         <v>208</v>
       </c>
@@ -16005,7 +16037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="129.6">
+    <row r="216" spans="1:20" ht="288">
       <c r="A216" s="20">
         <v>209</v>
       </c>
@@ -16039,7 +16071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="129.6">
+    <row r="217" spans="1:20" ht="273.60000000000002">
       <c r="A217" s="20">
         <v>210</v>
       </c>
@@ -16073,7 +16105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="129.6">
+    <row r="218" spans="1:20" ht="158.4">
       <c r="A218" s="20">
         <v>211</v>
       </c>
@@ -16107,7 +16139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="129.6">
+    <row r="219" spans="1:20" ht="288">
       <c r="A219" s="20">
         <v>212</v>
       </c>
@@ -16141,7 +16173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="129.6">
+    <row r="220" spans="1:20" ht="201.6">
       <c r="A220" s="20">
         <v>213</v>
       </c>
@@ -16175,7 +16207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="129.6">
+    <row r="221" spans="1:20" ht="230.4">
       <c r="A221" s="20">
         <v>214</v>
       </c>
@@ -16209,7 +16241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="129.6">
+    <row r="222" spans="1:20" ht="244.8">
       <c r="A222" s="20">
         <v>215</v>
       </c>
@@ -16243,7 +16275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="144">
+    <row r="223" spans="1:20" ht="244.8">
       <c r="A223" s="20">
         <v>216</v>
       </c>
@@ -16277,7 +16309,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="158.4">
+    <row r="224" spans="1:20" ht="244.8">
       <c r="A224" s="20">
         <v>217</v>
       </c>
@@ -16311,7 +16343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="43.2">
+    <row r="225" spans="1:20" ht="244.8">
       <c r="A225" s="20">
         <v>218</v>
       </c>
@@ -16345,7 +16377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="158.4">
+    <row r="226" spans="1:20" ht="244.8">
       <c r="A226" s="20">
         <v>219</v>
       </c>
@@ -16379,7 +16411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="158.4">
+    <row r="227" spans="1:20" ht="129.6">
       <c r="A227" s="20">
         <v>220</v>
       </c>
@@ -16413,7 +16445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="158.4">
+    <row r="228" spans="1:20" ht="259.2">
       <c r="A228" s="20">
         <v>221</v>
       </c>
@@ -16447,7 +16479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="158.4">
+    <row r="229" spans="1:20" ht="288">
       <c r="A229" s="20">
         <v>222</v>
       </c>
@@ -16481,7 +16513,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="115.2">
+    <row r="230" spans="1:20" ht="259.2">
       <c r="A230" s="20">
         <v>223</v>
       </c>
@@ -16515,7 +16547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="129.6" hidden="1">
+    <row r="231" spans="1:20" ht="216" hidden="1">
       <c r="A231" s="20">
         <v>224</v>
       </c>
@@ -16549,7 +16581,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="129.6" hidden="1">
+    <row r="232" spans="1:20" ht="288" hidden="1">
       <c r="A232" s="20">
         <v>225</v>
       </c>
@@ -16583,7 +16615,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="129.6" hidden="1">
+    <row r="233" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A233" s="20">
         <v>226</v>
       </c>
@@ -16617,7 +16649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="129.6" hidden="1">
+    <row r="234" spans="1:20" ht="158.4" hidden="1">
       <c r="A234" s="20">
         <v>227</v>
       </c>
@@ -16651,7 +16683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="129.6" hidden="1">
+    <row r="235" spans="1:20" ht="288" hidden="1">
       <c r="A235" s="20">
         <v>228</v>
       </c>
@@ -16685,7 +16717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="129.6" hidden="1">
+    <row r="236" spans="1:20" ht="201.6" hidden="1">
       <c r="A236" s="20">
         <v>229</v>
       </c>
@@ -16719,7 +16751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="115.2" hidden="1">
+    <row r="237" spans="1:20" ht="230.4" hidden="1">
       <c r="A237" s="20">
         <v>230</v>
       </c>
@@ -16753,7 +16785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="129.6" hidden="1">
+    <row r="238" spans="1:20" ht="244.8" hidden="1">
       <c r="A238" s="20">
         <v>231</v>
       </c>
@@ -16787,7 +16819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="129.6" hidden="1">
+    <row r="239" spans="1:20" ht="244.8" hidden="1">
       <c r="A239" s="20">
         <v>232</v>
       </c>
@@ -16821,7 +16853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="129.6" hidden="1">
+    <row r="240" spans="1:20" ht="244.8" hidden="1">
       <c r="A240" s="20">
         <v>233</v>
       </c>
@@ -16855,7 +16887,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="129.6" hidden="1">
+    <row r="241" spans="1:20" ht="244.8" hidden="1">
       <c r="A241" s="20">
         <v>234</v>
       </c>
@@ -16889,7 +16921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="129.6" hidden="1">
+    <row r="242" spans="1:20" ht="244.8" hidden="1">
       <c r="A242" s="20">
         <v>235</v>
       </c>
@@ -16957,7 +16989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="129.6" hidden="1">
+    <row r="244" spans="1:20" ht="259.2" hidden="1">
       <c r="A244" s="20">
         <v>237</v>
       </c>
@@ -16991,7 +17023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="129.6" hidden="1">
+    <row r="245" spans="1:20" ht="288" hidden="1">
       <c r="A245" s="20">
         <v>238</v>
       </c>
@@ -17025,7 +17057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="129.6" hidden="1">
+    <row r="246" spans="1:20" ht="259.2" hidden="1">
       <c r="A246" s="20">
         <v>239</v>
       </c>
@@ -17059,7 +17091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="144" hidden="1">
+    <row r="247" spans="1:20" ht="216" hidden="1">
       <c r="A247" s="20">
         <v>240</v>
       </c>
@@ -17093,7 +17125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="144" hidden="1">
+    <row r="248" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A248" s="20">
         <v>241</v>
       </c>
@@ -17127,7 +17159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="144" hidden="1">
+    <row r="249" spans="1:20" ht="288" hidden="1">
       <c r="A249" s="20">
         <v>242</v>
       </c>
@@ -17161,7 +17193,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="144" hidden="1">
+    <row r="250" spans="1:20" ht="172.8" hidden="1">
       <c r="A250" s="20">
         <v>243</v>
       </c>
@@ -17195,7 +17227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="144" hidden="1">
+    <row r="251" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A251" s="20">
         <v>244</v>
       </c>
@@ -17229,7 +17261,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="158.4" hidden="1">
+    <row r="252" spans="1:20" ht="201.6" hidden="1">
       <c r="A252" s="20">
         <v>245</v>
       </c>
@@ -17263,7 +17295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="43.2" hidden="1">
+    <row r="253" spans="1:20" ht="230.4" hidden="1">
       <c r="A253" s="20">
         <v>246</v>
       </c>
@@ -17297,7 +17329,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="144" hidden="1">
+    <row r="254" spans="1:20" ht="244.8" hidden="1">
       <c r="A254" s="20">
         <v>247</v>
       </c>
@@ -17331,7 +17363,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="129.6" hidden="1">
+    <row r="255" spans="1:20" ht="244.8" hidden="1">
       <c r="A255" s="20">
         <v>248</v>
       </c>
@@ -17365,7 +17397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="115.2" hidden="1">
+    <row r="256" spans="1:20" ht="244.8" hidden="1">
       <c r="A256" s="20">
         <v>249</v>
       </c>
@@ -17399,7 +17431,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="115.2" hidden="1">
+    <row r="257" spans="1:20" ht="244.8" hidden="1">
       <c r="A257" s="20">
         <v>250</v>
       </c>
@@ -17433,7 +17465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="129.6" hidden="1">
+    <row r="258" spans="1:20" ht="244.8" hidden="1">
       <c r="A258" s="20">
         <v>251</v>
       </c>
@@ -17501,7 +17533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="129.6" hidden="1">
+    <row r="260" spans="1:20" ht="259.2" hidden="1">
       <c r="A260" s="20">
         <v>253</v>
       </c>
@@ -17535,7 +17567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="129.6" hidden="1">
+    <row r="261" spans="1:20" ht="288" hidden="1">
       <c r="A261" s="20">
         <v>254</v>
       </c>
@@ -17569,7 +17601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="115.2" hidden="1">
+    <row r="262" spans="1:20" ht="259.2" hidden="1">
       <c r="A262" s="20">
         <v>255</v>
       </c>
@@ -17603,7 +17635,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="115.2" hidden="1">
+    <row r="263" spans="1:20" ht="216" hidden="1">
       <c r="A263" s="20">
         <v>256</v>
       </c>
@@ -17637,7 +17669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="129.6" hidden="1">
+    <row r="264" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A264" s="20">
         <v>257</v>
       </c>
@@ -17671,7 +17703,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="129.6" hidden="1">
+    <row r="265" spans="1:20" ht="288" hidden="1">
       <c r="A265" s="20">
         <v>258</v>
       </c>
@@ -17705,7 +17737,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="144" hidden="1">
+    <row r="266" spans="1:20" ht="172.8" hidden="1">
       <c r="A266" s="20">
         <v>259</v>
       </c>
@@ -17739,7 +17771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="129.6" hidden="1">
+    <row r="267" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A267" s="20">
         <v>260</v>
       </c>
@@ -17773,7 +17805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="115.2" hidden="1">
+    <row r="268" spans="1:20" ht="201.6" hidden="1">
       <c r="A268" s="20">
         <v>261</v>
       </c>
@@ -17807,7 +17839,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="115.2" hidden="1">
+    <row r="269" spans="1:20" ht="230.4" hidden="1">
       <c r="A269" s="20">
         <v>262</v>
       </c>
@@ -17841,7 +17873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="129.6" hidden="1">
+    <row r="270" spans="1:20" ht="244.8" hidden="1">
       <c r="A270" s="20">
         <v>263</v>
       </c>
@@ -17875,7 +17907,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="129.6" hidden="1">
+    <row r="271" spans="1:20" ht="244.8" hidden="1">
       <c r="A271" s="20">
         <v>264</v>
       </c>
@@ -17909,7 +17941,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="129.6" hidden="1">
+    <row r="272" spans="1:20" ht="244.8" hidden="1">
       <c r="A272" s="20">
         <v>265</v>
       </c>
@@ -17943,7 +17975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="144" hidden="1">
+    <row r="273" spans="1:20" ht="244.8" hidden="1">
       <c r="A273" s="20">
         <v>266</v>
       </c>
@@ -17977,7 +18009,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="158.4" hidden="1">
+    <row r="274" spans="1:20" ht="244.8" hidden="1">
       <c r="A274" s="20">
         <v>267</v>
       </c>
@@ -18011,7 +18043,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="43.2" hidden="1">
+    <row r="275" spans="1:20" ht="129.6" hidden="1">
       <c r="A275" s="20">
         <v>268</v>
       </c>
@@ -18045,7 +18077,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="158.4" hidden="1">
+    <row r="276" spans="1:20" ht="259.2" hidden="1">
       <c r="A276" s="20">
         <v>269</v>
       </c>
@@ -18079,7 +18111,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="158.4" hidden="1">
+    <row r="277" spans="1:20" ht="288" hidden="1">
       <c r="A277" s="20">
         <v>270</v>
       </c>
@@ -18113,7 +18145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="158.4" hidden="1">
+    <row r="278" spans="1:20" ht="259.2" hidden="1">
       <c r="A278" s="20">
         <v>271</v>
       </c>
@@ -18147,7 +18179,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="158.4">
+    <row r="279" spans="1:20" ht="216">
       <c r="A279" s="20">
         <v>272</v>
       </c>
@@ -18181,7 +18213,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="115.2">
+    <row r="280" spans="1:20" ht="288">
       <c r="A280" s="20">
         <v>273</v>
       </c>
@@ -18215,7 +18247,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="129.6">
+    <row r="281" spans="1:20" ht="273.60000000000002">
       <c r="A281" s="20">
         <v>274</v>
       </c>
@@ -18249,7 +18281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="129.6">
+    <row r="282" spans="1:20" ht="158.4">
       <c r="A282" s="20">
         <v>275</v>
       </c>
@@ -18283,7 +18315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="129.6">
+    <row r="283" spans="1:20" ht="288">
       <c r="A283" s="20">
         <v>276</v>
       </c>
@@ -18317,7 +18349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="129.6">
+    <row r="284" spans="1:20" ht="201.6">
       <c r="A284" s="20">
         <v>277</v>
       </c>
@@ -18351,7 +18383,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="129.6">
+    <row r="285" spans="1:20" ht="230.4">
       <c r="A285" s="20">
         <v>278</v>
       </c>
@@ -18385,7 +18417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="129.6">
+    <row r="286" spans="1:20" ht="244.8">
       <c r="A286" s="20">
         <v>279</v>
       </c>
@@ -18419,7 +18451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="129.6">
+    <row r="287" spans="1:20" ht="244.8">
       <c r="A287" s="20">
         <v>280</v>
       </c>
@@ -18453,7 +18485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="115.2">
+    <row r="288" spans="1:20" ht="244.8">
       <c r="A288" s="20">
         <v>281</v>
       </c>
@@ -18487,7 +18519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="115.2">
+    <row r="289" spans="1:20" ht="244.8">
       <c r="A289" s="20">
         <v>282</v>
       </c>
@@ -18521,7 +18553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="129.6">
+    <row r="290" spans="1:20" ht="244.8">
       <c r="A290" s="20">
         <v>283</v>
       </c>
@@ -18589,7 +18621,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="129.6">
+    <row r="292" spans="1:20" ht="259.2">
       <c r="A292" s="20">
         <v>285</v>
       </c>
@@ -18623,7 +18655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="129.6">
+    <row r="293" spans="1:20" ht="288">
       <c r="A293" s="20">
         <v>286</v>
       </c>
@@ -18657,7 +18689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="129.6">
+    <row r="294" spans="1:20" ht="259.2">
       <c r="A294" s="20">
         <v>287</v>
       </c>
@@ -18691,7 +18723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="129.6" hidden="1">
+    <row r="295" spans="1:20" ht="216" hidden="1">
       <c r="A295" s="20">
         <v>288</v>
       </c>
@@ -18725,7 +18757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="129.6" hidden="1">
+    <row r="296" spans="1:20" ht="288" hidden="1">
       <c r="A296" s="20">
         <v>289</v>
       </c>
@@ -18759,7 +18791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="129.6" hidden="1">
+    <row r="297" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A297" s="20">
         <v>290</v>
       </c>
@@ -18793,7 +18825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="129.6" hidden="1">
+    <row r="298" spans="1:20" ht="158.4" hidden="1">
       <c r="A298" s="20">
         <v>291</v>
       </c>
@@ -18827,7 +18859,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="144" hidden="1">
+    <row r="299" spans="1:20" ht="288" hidden="1">
       <c r="A299" s="20">
         <v>292</v>
       </c>
@@ -18861,7 +18893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="144" hidden="1">
+    <row r="300" spans="1:20" ht="201.6" hidden="1">
       <c r="A300" s="20">
         <v>293</v>
       </c>
@@ -18895,7 +18927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="144" hidden="1">
+    <row r="301" spans="1:20" ht="230.4" hidden="1">
       <c r="A301" s="20">
         <v>294</v>
       </c>
@@ -18929,7 +18961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="144" hidden="1">
+    <row r="302" spans="1:20" ht="244.8" hidden="1">
       <c r="A302" s="20">
         <v>295</v>
       </c>
@@ -18963,7 +18995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="144" hidden="1">
+    <row r="303" spans="1:20" ht="244.8" hidden="1">
       <c r="A303" s="20">
         <v>296</v>
       </c>
@@ -18997,7 +19029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="158.4" hidden="1">
+    <row r="304" spans="1:20" ht="244.8" hidden="1">
       <c r="A304" s="20">
         <v>297</v>
       </c>
@@ -19031,7 +19063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="43.2" hidden="1">
+    <row r="305" spans="1:20" ht="244.8" hidden="1">
       <c r="A305" s="20">
         <v>298</v>
       </c>
@@ -19065,7 +19097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="129.6" hidden="1">
+    <row r="306" spans="1:20" ht="244.8" hidden="1">
       <c r="A306" s="20">
         <v>299</v>
       </c>
@@ -19133,7 +19165,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="216" hidden="1">
+    <row r="308" spans="1:20" ht="259.2" hidden="1">
       <c r="A308" s="20">
         <v>301</v>
       </c>
@@ -19201,7 +19233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="310" spans="1:20" ht="259.2" hidden="1">
       <c r="A310" s="20">
         <v>303</v>
       </c>
@@ -19235,7 +19267,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="158.4" hidden="1">
+    <row r="311" spans="1:20" ht="216" hidden="1">
       <c r="A311" s="20">
         <v>304</v>
       </c>
@@ -19303,7 +19335,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="201.6" hidden="1">
+    <row r="313" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A313" s="20">
         <v>306</v>
       </c>
@@ -19337,7 +19369,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="230.4" hidden="1">
+    <row r="314" spans="1:20" ht="158.4" hidden="1">
       <c r="A314" s="20">
         <v>307</v>
       </c>
@@ -19371,7 +19403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="244.8" hidden="1">
+    <row r="315" spans="1:20" ht="288" hidden="1">
       <c r="A315" s="20">
         <v>308</v>
       </c>
@@ -19405,7 +19437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="244.8" hidden="1">
+    <row r="316" spans="1:20" ht="201.6" hidden="1">
       <c r="A316" s="20">
         <v>309</v>
       </c>
@@ -19439,7 +19471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="244.8" hidden="1">
+    <row r="317" spans="1:20" ht="230.4" hidden="1">
       <c r="A317" s="20">
         <v>310</v>
       </c>
@@ -19541,7 +19573,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="129.6" hidden="1">
+    <row r="320" spans="1:20" ht="244.8" hidden="1">
       <c r="A320" s="20">
         <v>313</v>
       </c>
@@ -19575,7 +19607,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="259.2" hidden="1">
+    <row r="321" spans="1:20" ht="244.8" hidden="1">
       <c r="A321" s="20">
         <v>314</v>
       </c>
@@ -19609,7 +19641,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="288" hidden="1">
+    <row r="322" spans="1:20" ht="244.8" hidden="1">
       <c r="A322" s="20">
         <v>315</v>
       </c>
@@ -19643,7 +19675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="259.2" hidden="1">
+    <row r="323" spans="1:20" ht="129.6" hidden="1">
       <c r="A323" s="20">
         <v>316</v>
       </c>
@@ -19677,7 +19709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="324" spans="1:20" ht="259.2" hidden="1">
       <c r="A324" s="20">
         <v>317</v>
       </c>
@@ -19711,7 +19743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="325" spans="1:20" ht="288" hidden="1">
       <c r="A325" s="20">
         <v>318</v>
       </c>
@@ -19745,7 +19777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="244.8" hidden="1">
+    <row r="326" spans="1:20" ht="259.2" hidden="1">
       <c r="A326" s="20">
         <v>319</v>
       </c>
@@ -19779,7 +19811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="327" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A327" s="20">
         <v>320</v>
       </c>
@@ -19813,7 +19845,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="216" hidden="1">
+    <row r="328" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A328" s="20">
         <v>321</v>
       </c>
@@ -19881,7 +19913,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="129.6" hidden="1">
+    <row r="330" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A330" s="20">
         <v>323</v>
       </c>
@@ -19915,7 +19947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="115.2">
+    <row r="331" spans="1:20" ht="302.39999999999998">
       <c r="A331" s="20">
         <v>324</v>
       </c>
@@ -19949,7 +19981,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="129.6">
+    <row r="332" spans="1:20" ht="259.2">
       <c r="A332" s="20">
         <v>325</v>
       </c>
@@ -19983,7 +20015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="129.6">
+    <row r="333" spans="1:20" ht="244.8">
       <c r="A333" s="20">
         <v>326</v>
       </c>
@@ -20017,7 +20049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="129.6">
+    <row r="334" spans="1:20" ht="273.60000000000002">
       <c r="A334" s="20">
         <v>327</v>
       </c>
@@ -20051,7 +20083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="129.6" hidden="1">
+    <row r="335" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A335" s="20">
         <v>328</v>
       </c>
@@ -20085,7 +20117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="129.6" hidden="1">
+    <row r="336" spans="1:20" ht="259.2" hidden="1">
       <c r="A336" s="20">
         <v>329</v>
       </c>
@@ -20119,7 +20151,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="129.6" hidden="1">
+    <row r="337" spans="1:20" ht="244.8" hidden="1">
       <c r="A337" s="20">
         <v>330</v>
       </c>
@@ -20153,7 +20185,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="129.6" hidden="1">
+    <row r="338" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A338" s="20">
         <v>331</v>
       </c>
@@ -20187,7 +20219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="129.6" hidden="1">
+    <row r="339" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A339" s="20">
         <v>332</v>
       </c>
@@ -20221,7 +20253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="129.6" hidden="1">
+    <row r="340" spans="1:20" ht="259.2" hidden="1">
       <c r="A340" s="20">
         <v>333</v>
       </c>
@@ -20255,7 +20287,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="129.6" hidden="1">
+    <row r="341" spans="1:20" ht="230.4" hidden="1">
       <c r="A341" s="20">
         <v>334</v>
       </c>
@@ -20289,7 +20321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="129.6" hidden="1">
+    <row r="342" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A342" s="20">
         <v>335</v>
       </c>
@@ -20323,7 +20355,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="129.6" hidden="1">
+    <row r="343" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A343" s="20">
         <v>336</v>
       </c>
@@ -20357,7 +20389,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="129.6" hidden="1">
+    <row r="344" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A344" s="20">
         <v>337</v>
       </c>
@@ -20391,7 +20423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="129.6" hidden="1">
+    <row r="345" spans="1:20" ht="244.8" hidden="1">
       <c r="A345" s="20">
         <v>338</v>
       </c>
@@ -20425,7 +20457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="129.6" hidden="1">
+    <row r="346" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A346" s="20">
         <v>339</v>
       </c>
@@ -20459,7 +20491,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="129.6">
+    <row r="347" spans="1:20" ht="302.39999999999998">
       <c r="A347" s="20">
         <v>340</v>
       </c>
@@ -20493,7 +20525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="129.6">
+    <row r="348" spans="1:20" ht="273.60000000000002">
       <c r="A348" s="20">
         <v>341</v>
       </c>
@@ -20527,7 +20559,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="129.6">
+    <row r="349" spans="1:20" ht="244.8">
       <c r="A349" s="20">
         <v>342</v>
       </c>
@@ -20561,7 +20593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="129.6">
+    <row r="350" spans="1:20" ht="273.60000000000002">
       <c r="A350" s="20">
         <v>343</v>
       </c>
@@ -20595,7 +20627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="129.6" hidden="1">
+    <row r="351" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A351" s="20">
         <v>344</v>
       </c>
@@ -20629,7 +20661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="129.6" hidden="1">
+    <row r="352" spans="1:20" ht="259.2" hidden="1">
       <c r="A352" s="20">
         <v>345</v>
       </c>
@@ -20663,7 +20695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="129.6" hidden="1">
+    <row r="353" spans="1:20" ht="230.4" hidden="1">
       <c r="A353" s="20">
         <v>346</v>
       </c>
@@ -20697,7 +20729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="129.6" hidden="1">
+    <row r="354" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A354" s="20">
         <v>347</v>
       </c>
@@ -20731,7 +20763,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="129.6" hidden="1">
+    <row r="355" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A355" s="20">
         <v>348</v>
       </c>
@@ -20765,7 +20797,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="129.6" hidden="1">
+    <row r="356" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A356" s="20">
         <v>349</v>
       </c>
@@ -20799,7 +20831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="129.6" hidden="1">
+    <row r="357" spans="1:20" ht="244.8" hidden="1">
       <c r="A357" s="20">
         <v>350</v>
       </c>
@@ -20833,7 +20865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="129.6" hidden="1">
+    <row r="358" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A358" s="20">
         <v>351</v>
       </c>
@@ -20867,7 +20899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="129.6" hidden="1">
+    <row r="359" spans="1:20" ht="216" hidden="1">
       <c r="A359" s="20">
         <v>352</v>
       </c>
@@ -20901,7 +20933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="129.6" hidden="1">
+    <row r="360" spans="1:20" ht="244.8" hidden="1">
       <c r="A360" s="20">
         <v>353</v>
       </c>
@@ -20935,7 +20967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="129.6">
+    <row r="361" spans="1:20" ht="216">
       <c r="A361" s="20">
         <v>354</v>
       </c>
@@ -20969,7 +21001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="129.6">
+    <row r="362" spans="1:20" ht="244.8">
       <c r="A362" s="20">
         <v>355</v>
       </c>
@@ -21003,7 +21035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="129.6" hidden="1">
+    <row r="363" spans="1:20" ht="216" hidden="1">
       <c r="A363" s="20">
         <v>356</v>
       </c>
@@ -21037,7 +21069,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="129.6" hidden="1">
+    <row r="364" spans="1:20" ht="244.8" hidden="1">
       <c r="A364" s="20">
         <v>357</v>
       </c>
@@ -21071,7 +21103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="129.6" hidden="1">
+    <row r="365" spans="1:20" ht="216" hidden="1">
       <c r="A365" s="20">
         <v>358</v>
       </c>
@@ -21105,7 +21137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="129.6" hidden="1">
+    <row r="366" spans="1:20" ht="244.8" hidden="1">
       <c r="A366" s="20">
         <v>359</v>
       </c>
@@ -21139,7 +21171,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="129.6" hidden="1">
+    <row r="367" spans="1:20" ht="216" hidden="1">
       <c r="A367" s="20">
         <v>360</v>
       </c>
@@ -21173,7 +21205,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="129.6" hidden="1">
+    <row r="368" spans="1:20" ht="244.8" hidden="1">
       <c r="A368" s="20">
         <v>361</v>
       </c>
@@ -21207,7 +21239,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="129.6">
+    <row r="369" spans="1:20" ht="216">
       <c r="A369" s="20">
         <v>362</v>
       </c>
@@ -21241,7 +21273,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="129.6">
+    <row r="370" spans="1:20" ht="244.8">
       <c r="A370" s="20">
         <v>363</v>
       </c>
@@ -21275,7 +21307,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="129.6" hidden="1">
+    <row r="371" spans="1:20" ht="216" hidden="1">
       <c r="A371" s="20">
         <v>364</v>
       </c>
@@ -21309,7 +21341,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="129.6" hidden="1">
+    <row r="372" spans="1:20" ht="244.8" hidden="1">
       <c r="A372" s="20">
         <v>365</v>
       </c>
@@ -21343,7 +21375,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="129.6" hidden="1">
+    <row r="373" spans="1:20" ht="216" hidden="1">
       <c r="A373" s="20">
         <v>366</v>
       </c>
@@ -21377,7 +21409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="129.6" hidden="1">
+    <row r="374" spans="1:20" ht="244.8" hidden="1">
       <c r="A374" s="20">
         <v>367</v>
       </c>
@@ -31041,7 +31073,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O230:O374 J308:J374 O186:O212 J214 L214:M214 O214 J211:J212 L211:M212 O216:O220 J222 L222:M222 O222 J219:J220 L219:M220 O224:O228 J227:J228 L227:M228 J186:J206 J216:J217 J224:J225 J230:J233 J235:J304 L36:M36 L216:M217 L224:M225 L230:M233 L235:M304 L308:M374 O12:O13 O20:O21 O82:O84 M28:M29 O44:O45 O52:O53 O60:O61 O68:O69 O28:O29 O36:O37 J36 L186:M206</xm:sqref>
+          <xm:sqref>O230:O374 J308:J374 O186:O212 J214 L214:M214 O214 J211:J212 L211:M212 O216:O220 J222 L222:M222 O222 J219:J220 L219:M220 O224:O228 J227:J228 L227:M228 J186:J206 J216:J217 J224:J225 J230:J233 J235:J304 L36:M36 L216:M217 L224:M225 L230:M233 L235:M304 L308:M374 O12:O13 O20:O21 O82:O84 M28:M29 O44:O45 L186:M206 O60:O61 O68:O69 O28:O29 O36:O37 J36 O53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Correzioni come da indicazioni 06-06-2023
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
+++ b/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\FSE_ACCREDITAMENTO\GATEWAY\S1#111PRAEZISIONX\PRAEZISION\ISOLABELLA\3.29.0.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10E702E-F21B-41D8-80B0-BE7555C06034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBBA46D-A94F-4471-B095-A921E9EBBBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3330" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="973">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3617,9 +3617,6 @@
     <t>SI'</t>
   </si>
   <si>
-    <t>Revisione dell'installazione cliente per correggere l'errore di configurazione.</t>
-  </si>
-  <si>
     <t>Errore di connessione.
 Contattare l'assistenza.</t>
   </si>
@@ -3629,12 +3626,6 @@
   </si>
   <si>
     <t>Viene mostrato l'errore generato dalla validazione.</t>
-  </si>
-  <si>
-    <t>modifica dei dati non corretti</t>
-  </si>
-  <si>
-    <t>Tentativi successivi.</t>
   </si>
   <si>
     <t>subject_application_id: ISOLABELLA</t>
@@ -4259,12 +4250,43 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
   </si>
+  <si>
+    <t>Viene chiesto a ll'utente di ritentare in seguito.
+Il documento rimane in una coda a disposizione del medico successivamente.</t>
+  </si>
+  <si>
+    <t>Revisione dell'installazione cliente per correggere l'errore di configurazione.
+Il documento rimane in una coda a disposizione del medico successivamente.</t>
+  </si>
+  <si>
+    <t>Modifica della codifica degli esami non corretti in backoffice.
+Il documento rimane in una coda a disposizione del medico successivamente.</t>
+  </si>
+  <si>
+    <t>Modifica dei dati non corretti in backoffice.
+Il documento rimane in una coda a disposizione del medico successivamente.</t>
+  </si>
+  <si>
+    <t>Aggiunta dati mancanti da parte del medico e re-invio in validazione contestualmente.</t>
+  </si>
+  <si>
+    <t>Modifica dei dati non corretti da parte del medico e re-invio in validazione contestualmente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifica dei dati non corretti in backoffice.
+Il documento rimane in una coda a disposizione del medico successivamente.
+</t>
+  </si>
+  <si>
+    <t>Revisione dell'installazione cliente per correggere l'errore di configurazione in backoffice.
+Il documento rimane in una coda a disposizione del medico successivamente.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4323,8 +4345,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4341,6 +4369,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4586,7 +4620,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4697,6 +4731,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7159,14 +7227,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="I324" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R326" sqref="R326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.33203125" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="43.44140625" customWidth="1"/>
     <col min="5" max="5" width="87.5546875" customWidth="1"/>
     <col min="6" max="6" width="21.88671875" customWidth="1"/>
@@ -7232,7 +7301,7 @@
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="44" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D3" s="36"/>
       <c r="F3" s="12"/>
@@ -7255,7 +7324,7 @@
       <c r="A4" s="40"/>
       <c r="B4" s="41"/>
       <c r="C4" s="44" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="4"/>
@@ -7279,7 +7348,7 @@
       <c r="A5" s="42"/>
       <c r="B5" s="43"/>
       <c r="C5" s="44" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D5" s="36"/>
       <c r="F5" s="12"/>
@@ -7417,7 +7486,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="158.4" hidden="1">
+    <row r="10" spans="1:20" ht="144" hidden="1">
       <c r="A10" s="20">
         <v>16</v>
       </c>
@@ -7451,7 +7520,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="158.4" hidden="1">
+    <row r="11" spans="1:20" ht="144" hidden="1">
       <c r="A11" s="20">
         <v>17</v>
       </c>
@@ -7519,7 +7588,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="158.4" hidden="1">
+    <row r="13" spans="1:20" ht="144" hidden="1">
       <c r="A13" s="20">
         <v>19</v>
       </c>
@@ -7553,7 +7622,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="158.4" hidden="1">
+    <row r="14" spans="1:20" ht="144" hidden="1">
       <c r="A14" s="20">
         <v>33</v>
       </c>
@@ -7567,7 +7636,7 @@
         <v>456</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -7587,7 +7656,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="144" hidden="1">
+    <row r="15" spans="1:20" ht="158.4" hidden="1">
       <c r="A15" s="20">
         <v>41</v>
       </c>
@@ -7601,7 +7670,7 @@
         <v>464</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -7621,7 +7690,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="144" hidden="1">
+    <row r="16" spans="1:20" ht="43.2" hidden="1">
       <c r="A16" s="20">
         <v>49</v>
       </c>
@@ -7725,7 +7794,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="144" hidden="1">
+    <row r="19" spans="1:20" ht="115.2" hidden="1">
       <c r="A19" s="20">
         <v>96</v>
       </c>
@@ -7759,7 +7828,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="144" hidden="1">
+    <row r="20" spans="1:20" ht="129.6" hidden="1">
       <c r="A20" s="20">
         <v>97</v>
       </c>
@@ -7861,7 +7930,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="144" hidden="1">
+    <row r="23" spans="1:20" ht="115.2" hidden="1">
       <c r="A23" s="20">
         <v>100</v>
       </c>
@@ -7895,7 +7964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="144" hidden="1">
+    <row r="24" spans="1:20" ht="129.6" hidden="1">
       <c r="A24" s="20">
         <v>101</v>
       </c>
@@ -7997,7 +8066,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="144" hidden="1">
+    <row r="27" spans="1:20" ht="115.2" hidden="1">
       <c r="A27" s="20">
         <v>104</v>
       </c>
@@ -8099,7 +8168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="144" hidden="1">
+    <row r="30" spans="1:20" ht="216" hidden="1">
       <c r="A30" s="20">
         <v>240</v>
       </c>
@@ -8133,7 +8202,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="144" hidden="1">
+    <row r="31" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A31" s="20">
         <v>241</v>
       </c>
@@ -8167,7 +8236,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="144" hidden="1">
+    <row r="32" spans="1:20" ht="288" hidden="1">
       <c r="A32" s="20">
         <v>242</v>
       </c>
@@ -8201,7 +8270,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="144" hidden="1">
+    <row r="33" spans="1:20" ht="172.8" hidden="1">
       <c r="A33" s="20">
         <v>243</v>
       </c>
@@ -8235,7 +8304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="144" hidden="1">
+    <row r="34" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A34" s="20">
         <v>244</v>
       </c>
@@ -8269,7 +8338,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="144" hidden="1">
+    <row r="35" spans="1:20" ht="201.6" hidden="1">
       <c r="A35" s="20">
         <v>245</v>
       </c>
@@ -8303,7 +8372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="144" hidden="1">
+    <row r="36" spans="1:20" ht="230.4" hidden="1">
       <c r="A36" s="20">
         <v>246</v>
       </c>
@@ -8337,7 +8406,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="144" hidden="1">
+    <row r="37" spans="1:20" ht="244.8" hidden="1">
       <c r="A37" s="20">
         <v>247</v>
       </c>
@@ -8371,7 +8440,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="144" hidden="1">
+    <row r="38" spans="1:20" ht="244.8" hidden="1">
       <c r="A38" s="20">
         <v>248</v>
       </c>
@@ -8405,7 +8474,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="144" hidden="1">
+    <row r="39" spans="1:20" ht="244.8" hidden="1">
       <c r="A39" s="20">
         <v>249</v>
       </c>
@@ -8439,7 +8508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="144" hidden="1">
+    <row r="40" spans="1:20" ht="244.8" hidden="1">
       <c r="A40" s="20">
         <v>250</v>
       </c>
@@ -8473,7 +8542,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="144" hidden="1">
+    <row r="41" spans="1:20" ht="244.8" hidden="1">
       <c r="A41" s="20">
         <v>251</v>
       </c>
@@ -8507,7 +8576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="144" hidden="1">
+    <row r="42" spans="1:20" ht="129.6" hidden="1">
       <c r="A42" s="20">
         <v>252</v>
       </c>
@@ -8541,7 +8610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="158.4" hidden="1">
+    <row r="43" spans="1:20" ht="259.2" hidden="1">
       <c r="A43" s="20">
         <v>253</v>
       </c>
@@ -8609,7 +8678,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="158.4" hidden="1">
+    <row r="45" spans="1:20" ht="259.2" hidden="1">
       <c r="A45" s="20">
         <v>255</v>
       </c>
@@ -8643,7 +8712,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="158.4" hidden="1">
+    <row r="46" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A46" s="20">
         <v>332</v>
       </c>
@@ -8677,7 +8746,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="158.4" hidden="1">
+    <row r="47" spans="1:20" ht="259.2" hidden="1">
       <c r="A47" s="20">
         <v>333</v>
       </c>
@@ -8711,7 +8780,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="158.4" hidden="1">
+    <row r="48" spans="1:20" ht="230.4" hidden="1">
       <c r="A48" s="20">
         <v>334</v>
       </c>
@@ -8745,7 +8814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="158.4" hidden="1">
+    <row r="49" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A49" s="20">
         <v>335</v>
       </c>
@@ -8779,7 +8848,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="158.4" hidden="1">
+    <row r="50" spans="1:20" ht="216" hidden="1">
       <c r="A50" s="20">
         <v>358</v>
       </c>
@@ -8813,7 +8882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="43.2" hidden="1">
+    <row r="51" spans="1:20" ht="244.8" hidden="1">
       <c r="A51" s="20">
         <v>359</v>
       </c>
@@ -8847,7 +8916,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="43.2" hidden="1">
+    <row r="52" spans="1:20" ht="158.4" hidden="1">
       <c r="A52" s="20">
         <v>1</v>
       </c>
@@ -8881,7 +8950,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="43.2" hidden="1">
+    <row r="53" spans="1:20" ht="158.4" hidden="1">
       <c r="A53" s="20">
         <v>2</v>
       </c>
@@ -8915,7 +8984,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="43.2" hidden="1">
+    <row r="54" spans="1:20" ht="158.4" hidden="1">
       <c r="A54" s="20">
         <v>3</v>
       </c>
@@ -8949,7 +9018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="43.2" hidden="1">
+    <row r="55" spans="1:20" ht="158.4" hidden="1">
       <c r="A55" s="20">
         <v>4</v>
       </c>
@@ -8983,7 +9052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="43.2" hidden="1">
+    <row r="56" spans="1:20" ht="158.4" hidden="1">
       <c r="A56" s="20">
         <v>5</v>
       </c>
@@ -9017,7 +9086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="43.2" hidden="1">
+    <row r="57" spans="1:20" ht="144" hidden="1">
       <c r="A57" s="20">
         <v>28</v>
       </c>
@@ -9031,7 +9100,7 @@
         <v>451</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="24"/>
@@ -9051,7 +9120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="43.2" hidden="1">
+    <row r="58" spans="1:20" ht="158.4" hidden="1">
       <c r="A58" s="20">
         <v>36</v>
       </c>
@@ -9065,7 +9134,7 @@
         <v>459</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="24"/>
@@ -9085,7 +9154,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="115.2" hidden="1">
+    <row r="59" spans="1:20" ht="43.2" hidden="1">
       <c r="A59" s="20">
         <v>44</v>
       </c>
@@ -9461,7 +9530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="129.6" hidden="1">
+    <row r="70" spans="1:20" ht="115.2" hidden="1">
       <c r="A70" s="20">
         <v>62</v>
       </c>
@@ -9495,7 +9564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="129.6" hidden="1">
+    <row r="71" spans="1:20" ht="158.4" hidden="1">
       <c r="A71" s="20">
         <v>191</v>
       </c>
@@ -9529,7 +9598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="129.6" hidden="1">
+    <row r="72" spans="1:20" ht="216" hidden="1">
       <c r="A72" s="20">
         <v>192</v>
       </c>
@@ -9563,7 +9632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="129.6" hidden="1">
+    <row r="73" spans="1:20" ht="288" hidden="1">
       <c r="A73" s="20">
         <v>193</v>
       </c>
@@ -9597,7 +9666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="129.6" hidden="1">
+    <row r="74" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A74" s="20">
         <v>194</v>
       </c>
@@ -9631,7 +9700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="129.6" hidden="1">
+    <row r="75" spans="1:20" ht="158.4" hidden="1">
       <c r="A75" s="20">
         <v>195</v>
       </c>
@@ -9665,7 +9734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="129.6" hidden="1">
+    <row r="76" spans="1:20" ht="288" hidden="1">
       <c r="A76" s="20">
         <v>196</v>
       </c>
@@ -9699,7 +9768,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="129.6" hidden="1">
+    <row r="77" spans="1:20" ht="201.6" hidden="1">
       <c r="A77" s="20">
         <v>197</v>
       </c>
@@ -9733,7 +9802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="129.6" hidden="1">
+    <row r="78" spans="1:20" ht="230.4" hidden="1">
       <c r="A78" s="20">
         <v>198</v>
       </c>
@@ -9767,7 +9836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="129.6" hidden="1">
+    <row r="79" spans="1:20" ht="244.8" hidden="1">
       <c r="A79" s="20">
         <v>199</v>
       </c>
@@ -9801,7 +9870,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="129.6" hidden="1">
+    <row r="80" spans="1:20" ht="244.8" hidden="1">
       <c r="A80" s="20">
         <v>200</v>
       </c>
@@ -9835,7 +9904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="129.6" hidden="1">
+    <row r="81" spans="1:20" ht="244.8" hidden="1">
       <c r="A81" s="20">
         <v>201</v>
       </c>
@@ -9869,7 +9938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="144" hidden="1">
+    <row r="82" spans="1:20" ht="244.8" hidden="1">
       <c r="A82" s="20">
         <v>202</v>
       </c>
@@ -9903,7 +9972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="129.6" hidden="1">
+    <row r="83" spans="1:20" ht="244.8" hidden="1">
       <c r="A83" s="20">
         <v>203</v>
       </c>
@@ -9937,7 +10006,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="115.2" hidden="1">
+    <row r="84" spans="1:20" ht="129.6" hidden="1">
       <c r="A84" s="20">
         <v>204</v>
       </c>
@@ -9971,7 +10040,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="115.2" hidden="1">
+    <row r="85" spans="1:20" ht="259.2" hidden="1">
       <c r="A85" s="20">
         <v>205</v>
       </c>
@@ -10005,7 +10074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="129.6" hidden="1">
+    <row r="86" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A86" s="20">
         <v>206</v>
       </c>
@@ -10039,7 +10108,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="129.6" hidden="1">
+    <row r="87" spans="1:20" ht="259.2" hidden="1">
       <c r="A87" s="20">
         <v>207</v>
       </c>
@@ -10073,7 +10142,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="129.6" hidden="1">
+    <row r="88" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A88" s="20">
         <v>320</v>
       </c>
@@ -10107,7 +10176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="129.6" hidden="1">
+    <row r="89" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A89" s="20">
         <v>321</v>
       </c>
@@ -10141,7 +10210,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="115.2" hidden="1">
+    <row r="90" spans="1:20" ht="244.8" hidden="1">
       <c r="A90" s="20">
         <v>322</v>
       </c>
@@ -10175,7 +10244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="115.2" hidden="1">
+    <row r="91" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A91" s="20">
         <v>323</v>
       </c>
@@ -10209,7 +10278,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="129.6" hidden="1">
+    <row r="92" spans="1:20" ht="216" hidden="1">
       <c r="A92" s="20">
         <v>352</v>
       </c>
@@ -10243,7 +10312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="129.6" hidden="1">
+    <row r="93" spans="1:20" ht="244.8" hidden="1">
       <c r="A93" s="20">
         <v>353</v>
       </c>
@@ -10297,13 +10366,13 @@
         <v>45076</v>
       </c>
       <c r="G94" s="24" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="H94" s="24" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="I94" s="24" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="J94" s="25" t="s">
         <v>776</v>
@@ -10343,13 +10412,13 @@
         <v>45076</v>
       </c>
       <c r="G95" s="24" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="H95" s="24" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="I95" s="24" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="J95" s="25" t="s">
         <v>776</v>
@@ -10389,13 +10458,13 @@
         <v>45076</v>
       </c>
       <c r="G96" s="24" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="H96" s="24" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="I96" s="24" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="J96" s="25" t="s">
         <v>776</v>
@@ -10435,13 +10504,13 @@
         <v>45076</v>
       </c>
       <c r="G97" s="24" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="H97" s="24" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="I97" s="24" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="J97" s="25" t="s">
         <v>776</v>
@@ -10475,16 +10544,16 @@
         <v>452</v>
       </c>
       <c r="E98" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F98" s="23">
         <v>45076</v>
       </c>
       <c r="G98" s="24" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="H98" s="24" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="I98" s="24" t="s">
         <v>775</v>
@@ -10500,13 +10569,13 @@
         <v>469</v>
       </c>
       <c r="N98" s="25" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O98" s="25" t="s">
-        <v>774</v>
+        <v>469</v>
       </c>
       <c r="P98" s="25" t="s">
-        <v>777</v>
+        <v>972</v>
       </c>
       <c r="Q98" s="25" t="s">
         <v>772</v>
@@ -10531,16 +10600,16 @@
         <v>460</v>
       </c>
       <c r="E99" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F99" s="23">
         <v>45076</v>
       </c>
       <c r="G99" s="24" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="H99" s="24" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="I99" s="24" t="s">
         <v>775</v>
@@ -10556,13 +10625,13 @@
         <v>469</v>
       </c>
       <c r="N99" s="25" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O99" s="25" t="s">
-        <v>774</v>
-      </c>
-      <c r="P99" s="25" t="s">
-        <v>777</v>
+        <v>469</v>
+      </c>
+      <c r="P99" s="46" t="s">
+        <v>966</v>
       </c>
       <c r="Q99" s="25" t="s">
         <v>772</v>
@@ -10573,7 +10642,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="43.2">
+    <row r="100" spans="1:20" ht="43.8" thickBot="1">
       <c r="A100" s="20">
         <v>45</v>
       </c>
@@ -10604,13 +10673,13 @@
         <v>469</v>
       </c>
       <c r="N100" s="25" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="O100" s="25" t="s">
-        <v>774</v>
-      </c>
-      <c r="P100" s="25" t="s">
-        <v>782</v>
+        <v>469</v>
+      </c>
+      <c r="P100" s="46" t="s">
+        <v>965</v>
       </c>
       <c r="Q100" s="25" t="s">
         <v>772</v>
@@ -10623,63 +10692,63 @@
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="129.6">
-      <c r="A101" s="20">
+    <row r="101" spans="1:20" s="55" customFormat="1" ht="130.19999999999999" thickBot="1">
+      <c r="A101" s="47">
         <v>63</v>
       </c>
-      <c r="B101" s="21" t="s">
+      <c r="B101" s="48" t="s">
         <v>404</v>
       </c>
-      <c r="C101" s="21" t="s">
+      <c r="C101" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D101" s="21" t="s">
+      <c r="D101" s="48" t="s">
         <v>499</v>
       </c>
-      <c r="E101" s="22" t="s">
+      <c r="E101" s="49" t="s">
         <v>500</v>
       </c>
-      <c r="F101" s="23">
+      <c r="F101" s="50">
         <v>45076</v>
       </c>
-      <c r="G101" s="24" t="s">
-        <v>892</v>
-      </c>
-      <c r="H101" s="24" t="s">
-        <v>893</v>
-      </c>
-      <c r="I101" s="24" t="s">
-        <v>894</v>
-      </c>
-      <c r="J101" s="25" t="s">
+      <c r="G101" s="51" t="s">
+        <v>889</v>
+      </c>
+      <c r="H101" s="51" t="s">
+        <v>890</v>
+      </c>
+      <c r="I101" s="51" t="s">
+        <v>891</v>
+      </c>
+      <c r="J101" s="46" t="s">
         <v>776</v>
       </c>
-      <c r="K101" s="25"/>
-      <c r="L101" s="25" t="s">
+      <c r="K101" s="46"/>
+      <c r="L101" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="M101" s="25" t="s">
+      <c r="M101" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="N101" s="25" t="s">
-        <v>780</v>
-      </c>
-      <c r="O101" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P101" s="25" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q101" s="25" t="s">
+      <c r="N101" s="46" t="s">
+        <v>779</v>
+      </c>
+      <c r="O101" s="46" t="s">
+        <v>774</v>
+      </c>
+      <c r="P101" s="56" t="s">
+        <v>969</v>
+      </c>
+      <c r="Q101" s="46" t="s">
         <v>772</v>
       </c>
-      <c r="R101" s="26"/>
-      <c r="S101" s="27"/>
-      <c r="T101" s="28" t="s">
+      <c r="R101" s="52"/>
+      <c r="S101" s="53"/>
+      <c r="T101" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="129.6">
+    <row r="102" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A102" s="20">
         <v>64</v>
       </c>
@@ -10699,10 +10768,10 @@
         <v>45076</v>
       </c>
       <c r="G102" s="24" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="H102" s="24" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="I102" s="24" t="s">
         <v>775</v>
@@ -10718,13 +10787,13 @@
         <v>469</v>
       </c>
       <c r="N102" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O102" s="25" t="s">
-        <v>469</v>
+        <v>774</v>
       </c>
       <c r="P102" s="25" t="s">
-        <v>781</v>
+        <v>970</v>
       </c>
       <c r="Q102" s="25" t="s">
         <v>772</v>
@@ -10735,63 +10804,63 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="129.6">
-      <c r="A103" s="20">
+    <row r="103" spans="1:20" s="55" customFormat="1" ht="130.19999999999999" thickBot="1">
+      <c r="A103" s="47">
         <v>65</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="48" t="s">
         <v>404</v>
       </c>
-      <c r="C103" s="21" t="s">
+      <c r="C103" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D103" s="21" t="s">
+      <c r="D103" s="48" t="s">
         <v>503</v>
       </c>
-      <c r="E103" s="22" t="s">
-        <v>931</v>
-      </c>
-      <c r="F103" s="23">
+      <c r="E103" s="49" t="s">
+        <v>928</v>
+      </c>
+      <c r="F103" s="50">
         <v>45076</v>
       </c>
-      <c r="G103" s="24" t="s">
-        <v>897</v>
-      </c>
-      <c r="H103" s="24" t="s">
-        <v>898</v>
-      </c>
-      <c r="I103" s="24" t="s">
-        <v>899</v>
-      </c>
-      <c r="J103" s="25" t="s">
+      <c r="G103" s="51" t="s">
+        <v>894</v>
+      </c>
+      <c r="H103" s="51" t="s">
+        <v>895</v>
+      </c>
+      <c r="I103" s="51" t="s">
+        <v>896</v>
+      </c>
+      <c r="J103" s="46" t="s">
         <v>776</v>
       </c>
-      <c r="K103" s="25"/>
-      <c r="L103" s="25" t="s">
+      <c r="K103" s="46"/>
+      <c r="L103" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="M103" s="25" t="s">
+      <c r="M103" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="N103" s="25" t="s">
-        <v>780</v>
-      </c>
-      <c r="O103" s="25" t="s">
+      <c r="N103" s="46" t="s">
+        <v>779</v>
+      </c>
+      <c r="O103" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="P103" s="25" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q103" s="25" t="s">
+      <c r="P103" s="46" t="s">
+        <v>967</v>
+      </c>
+      <c r="Q103" s="46" t="s">
         <v>772</v>
       </c>
-      <c r="R103" s="26"/>
-      <c r="S103" s="27"/>
-      <c r="T103" s="28" t="s">
+      <c r="R103" s="52"/>
+      <c r="S103" s="53"/>
+      <c r="T103" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="129.6">
+    <row r="104" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A104" s="20">
         <v>66</v>
       </c>
@@ -10805,19 +10874,19 @@
         <v>504</v>
       </c>
       <c r="E104" s="22" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="F104" s="23">
         <v>45076</v>
       </c>
       <c r="G104" s="24" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="H104" s="24" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="I104" s="24" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="J104" s="25" t="s">
         <v>776</v>
@@ -10830,13 +10899,13 @@
         <v>469</v>
       </c>
       <c r="N104" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O104" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P104" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P104" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q104" s="25" t="s">
         <v>772</v>
@@ -10847,7 +10916,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="129.6">
+    <row r="105" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A105" s="20">
         <v>67</v>
       </c>
@@ -10861,19 +10930,19 @@
         <v>505</v>
       </c>
       <c r="E105" s="22" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="F105" s="23">
         <v>45076</v>
       </c>
       <c r="G105" s="24" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="H105" s="24" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="I105" s="24" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="J105" s="25" t="s">
         <v>776</v>
@@ -10886,13 +10955,13 @@
         <v>469</v>
       </c>
       <c r="N105" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O105" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P105" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P105" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q105" s="25" t="s">
         <v>772</v>
@@ -10903,7 +10972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="129.6">
+    <row r="106" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A106" s="20">
         <v>68</v>
       </c>
@@ -10917,19 +10986,19 @@
         <v>506</v>
       </c>
       <c r="E106" s="22" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="F106" s="23">
         <v>45076</v>
       </c>
       <c r="G106" s="24" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="H106" s="24" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="I106" s="24" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="J106" s="25" t="s">
         <v>776</v>
@@ -10942,13 +11011,13 @@
         <v>469</v>
       </c>
       <c r="N106" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O106" s="25" t="s">
-        <v>469</v>
+        <v>774</v>
       </c>
       <c r="P106" s="25" t="s">
-        <v>781</v>
+        <v>970</v>
       </c>
       <c r="Q106" s="25" t="s">
         <v>772</v>
@@ -10959,7 +11028,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="129.6">
+    <row r="107" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A107" s="20">
         <v>69</v>
       </c>
@@ -10973,19 +11042,19 @@
         <v>507</v>
       </c>
       <c r="E107" s="22" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="F107" s="23">
         <v>45076</v>
       </c>
       <c r="G107" s="24" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="H107" s="24" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="I107" s="24" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="J107" s="25" t="s">
         <v>776</v>
@@ -10998,13 +11067,13 @@
         <v>469</v>
       </c>
       <c r="N107" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O107" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P107" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P107" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q107" s="25" t="s">
         <v>772</v>
@@ -11015,7 +11084,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="129.6">
+    <row r="108" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A108" s="20">
         <v>70</v>
       </c>
@@ -11029,19 +11098,19 @@
         <v>508</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="F108" s="23">
         <v>45076</v>
       </c>
       <c r="G108" s="24" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="H108" s="24" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="I108" s="24" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="J108" s="25" t="s">
         <v>776</v>
@@ -11054,13 +11123,13 @@
         <v>469</v>
       </c>
       <c r="N108" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O108" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P108" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P108" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q108" s="25" t="s">
         <v>772</v>
@@ -11071,7 +11140,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="129.6">
+    <row r="109" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A109" s="20">
         <v>71</v>
       </c>
@@ -11085,19 +11154,19 @@
         <v>509</v>
       </c>
       <c r="E109" s="22" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="F109" s="23">
         <v>45076</v>
       </c>
       <c r="G109" s="24" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="H109" s="24" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="J109" s="25" t="s">
         <v>776</v>
@@ -11110,13 +11179,13 @@
         <v>469</v>
       </c>
       <c r="N109" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O109" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P109" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P109" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q109" s="25" t="s">
         <v>772</v>
@@ -11127,7 +11196,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="129.6">
+    <row r="110" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A110" s="20">
         <v>72</v>
       </c>
@@ -11141,19 +11210,19 @@
         <v>510</v>
       </c>
       <c r="E110" s="22" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F110" s="23">
         <v>45076</v>
       </c>
       <c r="G110" s="24" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="H110" s="24" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="I110" s="24" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="J110" s="25" t="s">
         <v>776</v>
@@ -11166,13 +11235,13 @@
         <v>469</v>
       </c>
       <c r="N110" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O110" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P110" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P110" s="56" t="s">
+        <v>969</v>
       </c>
       <c r="Q110" s="25" t="s">
         <v>772</v>
@@ -11183,7 +11252,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="129.6">
+    <row r="111" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A111" s="20">
         <v>73</v>
       </c>
@@ -11197,19 +11266,19 @@
         <v>511</v>
       </c>
       <c r="E111" s="22" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="F111" s="23">
         <v>45076</v>
       </c>
       <c r="G111" s="24" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="H111" s="24" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="I111" s="24" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="J111" s="25" t="s">
         <v>776</v>
@@ -11222,13 +11291,13 @@
         <v>469</v>
       </c>
       <c r="N111" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O111" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P111" s="25" t="s">
-        <v>781</v>
+        <v>971</v>
       </c>
       <c r="Q111" s="25" t="s">
         <v>772</v>
@@ -11253,19 +11322,19 @@
         <v>512</v>
       </c>
       <c r="E112" s="22" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="F112" s="23">
         <v>45076</v>
       </c>
       <c r="G112" s="24" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="H112" s="24" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="J112" s="25" t="s">
         <v>776</v>
@@ -11278,13 +11347,13 @@
         <v>469</v>
       </c>
       <c r="N112" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O112" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P112" s="25" t="s">
-        <v>781</v>
+        <v>971</v>
       </c>
       <c r="Q112" s="25" t="s">
         <v>772</v>
@@ -11295,7 +11364,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="144" hidden="1">
+    <row r="113" spans="1:20" ht="216" hidden="1">
       <c r="A113" s="20">
         <v>208</v>
       </c>
@@ -11329,7 +11398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="129.6" hidden="1">
+    <row r="114" spans="1:20" ht="288" hidden="1">
       <c r="A114" s="20">
         <v>209</v>
       </c>
@@ -11363,7 +11432,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="129.6" hidden="1">
+    <row r="115" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A115" s="20">
         <v>210</v>
       </c>
@@ -11397,7 +11466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="129.6" hidden="1">
+    <row r="116" spans="1:20" ht="158.4" hidden="1">
       <c r="A116" s="20">
         <v>211</v>
       </c>
@@ -11431,7 +11500,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="115.2" hidden="1">
+    <row r="117" spans="1:20" ht="288" hidden="1">
       <c r="A117" s="20">
         <v>212</v>
       </c>
@@ -11465,7 +11534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="129.6" hidden="1">
+    <row r="118" spans="1:20" ht="201.6" hidden="1">
       <c r="A118" s="20">
         <v>213</v>
       </c>
@@ -11499,7 +11568,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="129.6" hidden="1">
+    <row r="119" spans="1:20" ht="230.4" hidden="1">
       <c r="A119" s="20">
         <v>214</v>
       </c>
@@ -11533,7 +11602,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="129.6" hidden="1">
+    <row r="120" spans="1:20" ht="244.8" hidden="1">
       <c r="A120" s="20">
         <v>215</v>
       </c>
@@ -11567,7 +11636,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="129.6" hidden="1">
+    <row r="121" spans="1:20" ht="244.8" hidden="1">
       <c r="A121" s="20">
         <v>216</v>
       </c>
@@ -11601,7 +11670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="129.6" hidden="1">
+    <row r="122" spans="1:20" ht="244.8" hidden="1">
       <c r="A122" s="20">
         <v>217</v>
       </c>
@@ -11635,7 +11704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="129.6" hidden="1">
+    <row r="123" spans="1:20" ht="244.8" hidden="1">
       <c r="A123" s="20">
         <v>218</v>
       </c>
@@ -11669,7 +11738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="129.6" hidden="1">
+    <row r="124" spans="1:20" ht="244.8" hidden="1">
       <c r="A124" s="20">
         <v>219</v>
       </c>
@@ -11737,7 +11806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="129.6" hidden="1">
+    <row r="126" spans="1:20" ht="259.2" hidden="1">
       <c r="A126" s="20">
         <v>221</v>
       </c>
@@ -11771,7 +11840,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="129.6" hidden="1">
+    <row r="127" spans="1:20" ht="288" hidden="1">
       <c r="A127" s="20">
         <v>222</v>
       </c>
@@ -11805,7 +11874,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="129.6" hidden="1">
+    <row r="128" spans="1:20" ht="259.2" hidden="1">
       <c r="A128" s="20">
         <v>223</v>
       </c>
@@ -11839,7 +11908,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="115.2" hidden="1">
+    <row r="129" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A129" s="20">
         <v>324</v>
       </c>
@@ -11873,7 +11942,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="115.2" hidden="1">
+    <row r="130" spans="1:20" ht="259.2" hidden="1">
       <c r="A130" s="20">
         <v>325</v>
       </c>
@@ -11907,7 +11976,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="115.2" hidden="1">
+    <row r="131" spans="1:20" ht="244.8" hidden="1">
       <c r="A131" s="20">
         <v>326</v>
       </c>
@@ -11941,7 +12010,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="129.6" hidden="1">
+    <row r="132" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A132" s="20">
         <v>327</v>
       </c>
@@ -11975,7 +12044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="115.2" hidden="1">
+    <row r="133" spans="1:20" ht="216" hidden="1">
       <c r="A133" s="20">
         <v>354</v>
       </c>
@@ -12009,7 +12078,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="115.2" hidden="1">
+    <row r="134" spans="1:20" ht="244.8" hidden="1">
       <c r="A134" s="20">
         <v>355</v>
       </c>
@@ -12043,7 +12112,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="115.2" hidden="1">
+    <row r="135" spans="1:20" ht="144" hidden="1">
       <c r="A135" s="20">
         <v>30</v>
       </c>
@@ -12057,7 +12126,7 @@
         <v>453</v>
       </c>
       <c r="E135" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F135" s="23"/>
       <c r="G135" s="24"/>
@@ -12077,7 +12146,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="129.6" hidden="1">
+    <row r="136" spans="1:20" ht="158.4" hidden="1">
       <c r="A136" s="20">
         <v>38</v>
       </c>
@@ -12091,7 +12160,7 @@
         <v>461</v>
       </c>
       <c r="E136" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F136" s="23"/>
       <c r="G136" s="24"/>
@@ -12111,7 +12180,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="115.2" hidden="1">
+    <row r="137" spans="1:20" ht="43.2" hidden="1">
       <c r="A137" s="20">
         <v>46</v>
       </c>
@@ -12147,7 +12216,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="115.2" hidden="1">
+    <row r="138" spans="1:20" ht="158.4" hidden="1">
       <c r="A138" s="20">
         <v>170</v>
       </c>
@@ -12181,7 +12250,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="115.2" hidden="1">
+    <row r="139" spans="1:20" ht="158.4" hidden="1">
       <c r="A139" s="20">
         <v>171</v>
       </c>
@@ -12215,7 +12284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="129.6" hidden="1">
+    <row r="140" spans="1:20" ht="158.4" hidden="1">
       <c r="A140" s="20">
         <v>172</v>
       </c>
@@ -12249,7 +12318,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="115.2" hidden="1">
+    <row r="141" spans="1:20" ht="158.4" hidden="1">
       <c r="A141" s="20">
         <v>173</v>
       </c>
@@ -12317,7 +12386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="115.2" hidden="1">
+    <row r="143" spans="1:20" ht="129.6" hidden="1">
       <c r="A143" s="20">
         <v>175</v>
       </c>
@@ -12385,7 +12454,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="115.2" hidden="1">
+    <row r="145" spans="1:20" ht="129.6" hidden="1">
       <c r="A145" s="20">
         <v>177</v>
       </c>
@@ -12419,7 +12488,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="115.2" hidden="1">
+    <row r="146" spans="1:20" ht="129.6" hidden="1">
       <c r="A146" s="20">
         <v>178</v>
       </c>
@@ -12453,7 +12522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="115.2" hidden="1">
+    <row r="147" spans="1:20" ht="129.6" hidden="1">
       <c r="A147" s="20">
         <v>179</v>
       </c>
@@ -12555,7 +12624,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="115.2" hidden="1">
+    <row r="150" spans="1:20" ht="129.6" hidden="1">
       <c r="A150" s="20">
         <v>182</v>
       </c>
@@ -12589,7 +12658,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="115.2" hidden="1">
+    <row r="151" spans="1:20" ht="129.6" hidden="1">
       <c r="A151" s="20">
         <v>183</v>
       </c>
@@ -12691,7 +12760,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="158.4" hidden="1">
+    <row r="154" spans="1:20" ht="129.6" hidden="1">
       <c r="A154" s="20">
         <v>186</v>
       </c>
@@ -12725,7 +12794,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="158.4" hidden="1">
+    <row r="155" spans="1:20" ht="129.6" hidden="1">
       <c r="A155" s="20">
         <v>187</v>
       </c>
@@ -12759,7 +12828,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="158.4" hidden="1">
+    <row r="156" spans="1:20" ht="129.6" hidden="1">
       <c r="A156" s="20">
         <v>188</v>
       </c>
@@ -12793,7 +12862,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="158.4" hidden="1">
+    <row r="157" spans="1:20" ht="129.6" hidden="1">
       <c r="A157" s="20">
         <v>189</v>
       </c>
@@ -12827,7 +12896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="115.2" hidden="1">
+    <row r="158" spans="1:20" ht="129.6" hidden="1">
       <c r="A158" s="20">
         <v>190</v>
       </c>
@@ -12861,7 +12930,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="129.6" hidden="1">
+    <row r="159" spans="1:20" ht="216" hidden="1">
       <c r="A159" s="20">
         <v>304</v>
       </c>
@@ -12895,7 +12964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="129.6" hidden="1">
+    <row r="160" spans="1:20" ht="288" hidden="1">
       <c r="A160" s="20">
         <v>305</v>
       </c>
@@ -12929,7 +12998,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="129.6" hidden="1">
+    <row r="161" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A161" s="20">
         <v>306</v>
       </c>
@@ -12963,7 +13032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="129.6" hidden="1">
+    <row r="162" spans="1:20" ht="158.4" hidden="1">
       <c r="A162" s="20">
         <v>307</v>
       </c>
@@ -12997,7 +13066,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="129.6" hidden="1">
+    <row r="163" spans="1:20" ht="288" hidden="1">
       <c r="A163" s="20">
         <v>308</v>
       </c>
@@ -13031,7 +13100,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="129.6" hidden="1">
+    <row r="164" spans="1:20" ht="201.6" hidden="1">
       <c r="A164" s="20">
         <v>309</v>
       </c>
@@ -13065,7 +13134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="129.6" hidden="1">
+    <row r="165" spans="1:20" ht="230.4" hidden="1">
       <c r="A165" s="20">
         <v>310</v>
       </c>
@@ -13099,7 +13168,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="115.2" hidden="1">
+    <row r="166" spans="1:20" ht="244.8" hidden="1">
       <c r="A166" s="20">
         <v>311</v>
       </c>
@@ -13133,7 +13202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="115.2" hidden="1">
+    <row r="167" spans="1:20" ht="244.8" hidden="1">
       <c r="A167" s="20">
         <v>312</v>
       </c>
@@ -13167,7 +13236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="129.6" hidden="1">
+    <row r="168" spans="1:20" ht="244.8" hidden="1">
       <c r="A168" s="20">
         <v>313</v>
       </c>
@@ -13201,7 +13270,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="129.6" hidden="1">
+    <row r="169" spans="1:20" ht="244.8" hidden="1">
       <c r="A169" s="20">
         <v>314</v>
       </c>
@@ -13235,7 +13304,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="129.6" hidden="1">
+    <row r="170" spans="1:20" ht="244.8" hidden="1">
       <c r="A170" s="20">
         <v>315</v>
       </c>
@@ -13303,7 +13372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="129.6" hidden="1">
+    <row r="172" spans="1:20" ht="259.2" hidden="1">
       <c r="A172" s="20">
         <v>317</v>
       </c>
@@ -13337,7 +13406,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="129.6" hidden="1">
+    <row r="173" spans="1:20" ht="288" hidden="1">
       <c r="A173" s="20">
         <v>318</v>
       </c>
@@ -13371,7 +13440,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="129.6" hidden="1">
+    <row r="174" spans="1:20" ht="259.2" hidden="1">
       <c r="A174" s="20">
         <v>319</v>
       </c>
@@ -13405,7 +13474,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="129.6" hidden="1">
+    <row r="175" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A175" s="20">
         <v>348</v>
       </c>
@@ -13439,7 +13508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="129.6" hidden="1">
+    <row r="176" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A176" s="20">
         <v>349</v>
       </c>
@@ -13473,7 +13542,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="158.4" hidden="1">
+    <row r="177" spans="1:20" ht="244.8" hidden="1">
       <c r="A177" s="20">
         <v>350</v>
       </c>
@@ -13507,7 +13576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="158.4" hidden="1">
+    <row r="178" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A178" s="20">
         <v>351</v>
       </c>
@@ -13541,7 +13610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="158.4" hidden="1">
+    <row r="179" spans="1:20" ht="216" hidden="1">
       <c r="A179" s="20">
         <v>366</v>
       </c>
@@ -13575,7 +13644,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="158.4" hidden="1">
+    <row r="180" spans="1:20" ht="244.8" hidden="1">
       <c r="A180" s="20">
         <v>367</v>
       </c>
@@ -13609,7 +13678,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="115.2" hidden="1">
+    <row r="181" spans="1:20" ht="144" hidden="1">
       <c r="A181" s="20">
         <v>11</v>
       </c>
@@ -13643,7 +13712,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="129.6" hidden="1">
+    <row r="182" spans="1:20" ht="144" hidden="1">
       <c r="A182" s="20">
         <v>12</v>
       </c>
@@ -13677,7 +13746,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="129.6" hidden="1">
+    <row r="183" spans="1:20" ht="144" hidden="1">
       <c r="A183" s="20">
         <v>13</v>
       </c>
@@ -13711,7 +13780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="129.6" hidden="1">
+    <row r="184" spans="1:20" ht="144" hidden="1">
       <c r="A184" s="20">
         <v>14</v>
       </c>
@@ -13745,7 +13814,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="129.6" hidden="1">
+    <row r="185" spans="1:20" ht="144" hidden="1">
       <c r="A185" s="20">
         <v>31</v>
       </c>
@@ -13759,7 +13828,7 @@
         <v>454</v>
       </c>
       <c r="E185" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F185" s="23"/>
       <c r="G185" s="24"/>
@@ -13779,7 +13848,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="129.6" hidden="1">
+    <row r="186" spans="1:20" ht="158.4" hidden="1">
       <c r="A186" s="20">
         <v>39</v>
       </c>
@@ -13793,7 +13862,7 @@
         <v>462</v>
       </c>
       <c r="E186" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F186" s="23"/>
       <c r="G186" s="24"/>
@@ -13813,7 +13882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="129.6" hidden="1">
+    <row r="187" spans="1:20" ht="43.2" hidden="1">
       <c r="A187" s="20">
         <v>47</v>
       </c>
@@ -13849,7 +13918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="115.2" hidden="1">
+    <row r="188" spans="1:20" ht="144" hidden="1">
       <c r="A188" s="20">
         <v>75</v>
       </c>
@@ -13917,7 +13986,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="129.6" hidden="1">
+    <row r="190" spans="1:20" ht="115.2" hidden="1">
       <c r="A190" s="20">
         <v>77</v>
       </c>
@@ -13951,7 +14020,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="129.6" hidden="1">
+    <row r="191" spans="1:20" ht="115.2" hidden="1">
       <c r="A191" s="20">
         <v>78</v>
       </c>
@@ -14121,7 +14190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="129.6" hidden="1">
+    <row r="196" spans="1:20" ht="115.2" hidden="1">
       <c r="A196" s="20">
         <v>83</v>
       </c>
@@ -14155,7 +14224,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="129.6" hidden="1">
+    <row r="197" spans="1:20" ht="115.2" hidden="1">
       <c r="A197" s="20">
         <v>84</v>
       </c>
@@ -14189,7 +14258,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="158.4" hidden="1">
+    <row r="198" spans="1:20" ht="129.6" hidden="1">
       <c r="A198" s="20">
         <v>85</v>
       </c>
@@ -14223,7 +14292,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="216" hidden="1">
+    <row r="199" spans="1:20" ht="129.6" hidden="1">
       <c r="A199" s="20">
         <v>86</v>
       </c>
@@ -14257,7 +14326,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="288" hidden="1">
+    <row r="200" spans="1:20" ht="144" hidden="1">
       <c r="A200" s="20">
         <v>87</v>
       </c>
@@ -14291,7 +14360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="201" spans="1:20" ht="129.6" hidden="1">
       <c r="A201" s="20">
         <v>88</v>
       </c>
@@ -14325,7 +14394,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="158.4" hidden="1">
+    <row r="202" spans="1:20" ht="115.2" hidden="1">
       <c r="A202" s="20">
         <v>89</v>
       </c>
@@ -14359,7 +14428,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="288" hidden="1">
+    <row r="203" spans="1:20" ht="115.2" hidden="1">
       <c r="A203" s="20">
         <v>90</v>
       </c>
@@ -14393,7 +14462,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="201.6" hidden="1">
+    <row r="204" spans="1:20" ht="129.6" hidden="1">
       <c r="A204" s="20">
         <v>91</v>
       </c>
@@ -14427,7 +14496,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="230.4" hidden="1">
+    <row r="205" spans="1:20" ht="129.6" hidden="1">
       <c r="A205" s="20">
         <v>92</v>
       </c>
@@ -14461,7 +14530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="244.8" hidden="1">
+    <row r="206" spans="1:20" ht="129.6" hidden="1">
       <c r="A206" s="20">
         <v>93</v>
       </c>
@@ -14495,7 +14564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="244.8" hidden="1">
+    <row r="207" spans="1:20" ht="216" hidden="1">
       <c r="A207" s="20">
         <v>224</v>
       </c>
@@ -14529,7 +14598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="244.8" hidden="1">
+    <row r="208" spans="1:20" ht="288" hidden="1">
       <c r="A208" s="20">
         <v>225</v>
       </c>
@@ -14563,7 +14632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="244.8" hidden="1">
+    <row r="209" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A209" s="20">
         <v>226</v>
       </c>
@@ -14597,7 +14666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="244.8" hidden="1">
+    <row r="210" spans="1:20" ht="158.4" hidden="1">
       <c r="A210" s="20">
         <v>227</v>
       </c>
@@ -14631,7 +14700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="129.6" hidden="1">
+    <row r="211" spans="1:20" ht="288" hidden="1">
       <c r="A211" s="20">
         <v>228</v>
       </c>
@@ -14665,7 +14734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="259.2" hidden="1">
+    <row r="212" spans="1:20" ht="201.6" hidden="1">
       <c r="A212" s="20">
         <v>229</v>
       </c>
@@ -14699,7 +14768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="213" spans="1:20" ht="230.4" hidden="1">
       <c r="A213" s="20">
         <v>230</v>
       </c>
@@ -14733,7 +14802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="259.2" hidden="1">
+    <row r="214" spans="1:20" ht="244.8" hidden="1">
       <c r="A214" s="20">
         <v>231</v>
       </c>
@@ -14767,7 +14836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="216" hidden="1">
+    <row r="215" spans="1:20" ht="244.8" hidden="1">
       <c r="A215" s="20">
         <v>232</v>
       </c>
@@ -14801,7 +14870,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="288" hidden="1">
+    <row r="216" spans="1:20" ht="244.8" hidden="1">
       <c r="A216" s="20">
         <v>233</v>
       </c>
@@ -14835,7 +14904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="217" spans="1:20" ht="244.8" hidden="1">
       <c r="A217" s="20">
         <v>234</v>
       </c>
@@ -14869,7 +14938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="158.4" hidden="1">
+    <row r="218" spans="1:20" ht="244.8" hidden="1">
       <c r="A218" s="20">
         <v>235</v>
       </c>
@@ -14903,7 +14972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="288" hidden="1">
+    <row r="219" spans="1:20" ht="129.6" hidden="1">
       <c r="A219" s="20">
         <v>236</v>
       </c>
@@ -14937,7 +15006,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="201.6" hidden="1">
+    <row r="220" spans="1:20" ht="259.2" hidden="1">
       <c r="A220" s="20">
         <v>237</v>
       </c>
@@ -14971,7 +15040,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="230.4" hidden="1">
+    <row r="221" spans="1:20" ht="288" hidden="1">
       <c r="A221" s="20">
         <v>238</v>
       </c>
@@ -15005,7 +15074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="244.8" hidden="1">
+    <row r="222" spans="1:20" ht="259.2" hidden="1">
       <c r="A222" s="20">
         <v>239</v>
       </c>
@@ -15039,7 +15108,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="244.8" hidden="1">
+    <row r="223" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A223" s="20">
         <v>328</v>
       </c>
@@ -15073,7 +15142,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="244.8" hidden="1">
+    <row r="224" spans="1:20" ht="259.2" hidden="1">
       <c r="A224" s="20">
         <v>329</v>
       </c>
@@ -15141,7 +15210,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="244.8" hidden="1">
+    <row r="226" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A226" s="20">
         <v>331</v>
       </c>
@@ -15175,7 +15244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="129.6" hidden="1">
+    <row r="227" spans="1:20" ht="216" hidden="1">
       <c r="A227" s="20">
         <v>356</v>
       </c>
@@ -15209,7 +15278,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="259.2" hidden="1">
+    <row r="228" spans="1:20" ht="244.8" hidden="1">
       <c r="A228" s="20">
         <v>357</v>
       </c>
@@ -15243,7 +15312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="288" hidden="1">
+    <row r="229" spans="1:20" ht="144" hidden="1">
       <c r="A229" s="20">
         <v>32</v>
       </c>
@@ -15257,7 +15326,7 @@
         <v>455</v>
       </c>
       <c r="E229" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F229" s="23"/>
       <c r="G229" s="24"/>
@@ -15277,7 +15346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="259.2" hidden="1">
+    <row r="230" spans="1:20" ht="158.4" hidden="1">
       <c r="A230" s="20">
         <v>40</v>
       </c>
@@ -15291,7 +15360,7 @@
         <v>463</v>
       </c>
       <c r="E230" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F230" s="23"/>
       <c r="G230" s="24"/>
@@ -15311,7 +15380,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="216" hidden="1">
+    <row r="231" spans="1:20" ht="43.2" hidden="1">
       <c r="A231" s="20">
         <v>48</v>
       </c>
@@ -15347,7 +15416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="288" hidden="1">
+    <row r="232" spans="1:20" ht="158.4" hidden="1">
       <c r="A232" s="20">
         <v>147</v>
       </c>
@@ -15381,7 +15450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="233" spans="1:20" ht="158.4" hidden="1">
       <c r="A233" s="20">
         <v>148</v>
       </c>
@@ -15449,7 +15518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="288" hidden="1">
+    <row r="235" spans="1:20" ht="158.4" hidden="1">
       <c r="A235" s="20">
         <v>150</v>
       </c>
@@ -15483,7 +15552,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="201.6" hidden="1">
+    <row r="236" spans="1:20" ht="115.2" hidden="1">
       <c r="A236" s="20">
         <v>151</v>
       </c>
@@ -15517,7 +15586,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="230.4" hidden="1">
+    <row r="237" spans="1:20" ht="129.6" hidden="1">
       <c r="A237" s="20">
         <v>152</v>
       </c>
@@ -15551,7 +15620,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="244.8" hidden="1">
+    <row r="238" spans="1:20" ht="129.6" hidden="1">
       <c r="A238" s="20">
         <v>153</v>
       </c>
@@ -15585,7 +15654,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="244.8" hidden="1">
+    <row r="239" spans="1:20" ht="129.6" hidden="1">
       <c r="A239" s="20">
         <v>154</v>
       </c>
@@ -15619,7 +15688,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="244.8" hidden="1">
+    <row r="240" spans="1:20" ht="129.6" hidden="1">
       <c r="A240" s="20">
         <v>155</v>
       </c>
@@ -15653,7 +15722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="244.8" hidden="1">
+    <row r="241" spans="1:20" ht="129.6" hidden="1">
       <c r="A241" s="20">
         <v>156</v>
       </c>
@@ -15687,7 +15756,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="244.8" hidden="1">
+    <row r="242" spans="1:20" ht="129.6" hidden="1">
       <c r="A242" s="20">
         <v>157</v>
       </c>
@@ -15755,7 +15824,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="259.2" hidden="1">
+    <row r="244" spans="1:20" ht="115.2" hidden="1">
       <c r="A244" s="20">
         <v>159</v>
       </c>
@@ -15789,7 +15858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="288" hidden="1">
+    <row r="245" spans="1:20" ht="115.2" hidden="1">
       <c r="A245" s="20">
         <v>160</v>
       </c>
@@ -15823,7 +15892,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="259.2" hidden="1">
+    <row r="246" spans="1:20" ht="129.6" hidden="1">
       <c r="A246" s="20">
         <v>161</v>
       </c>
@@ -15857,7 +15926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="216" hidden="1">
+    <row r="247" spans="1:20" ht="129.6" hidden="1">
       <c r="A247" s="20">
         <v>162</v>
       </c>
@@ -15891,7 +15960,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="248" spans="1:20" ht="129.6" hidden="1">
       <c r="A248" s="20">
         <v>163</v>
       </c>
@@ -15925,7 +15994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="288" hidden="1">
+    <row r="249" spans="1:20" ht="129.6" hidden="1">
       <c r="A249" s="20">
         <v>164</v>
       </c>
@@ -15959,7 +16028,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="172.8" hidden="1">
+    <row r="250" spans="1:20" ht="129.6" hidden="1">
       <c r="A250" s="20">
         <v>165</v>
       </c>
@@ -15993,7 +16062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="251" spans="1:20" ht="129.6" hidden="1">
       <c r="A251" s="20">
         <v>166</v>
       </c>
@@ -16027,7 +16096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="201.6" hidden="1">
+    <row r="252" spans="1:20" ht="129.6" hidden="1">
       <c r="A252" s="20">
         <v>167</v>
       </c>
@@ -16061,7 +16130,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="230.4" hidden="1">
+    <row r="253" spans="1:20" ht="129.6" hidden="1">
       <c r="A253" s="20">
         <v>168</v>
       </c>
@@ -16095,7 +16164,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="244.8" hidden="1">
+    <row r="254" spans="1:20" ht="129.6" hidden="1">
       <c r="A254" s="20">
         <v>169</v>
       </c>
@@ -16129,7 +16198,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="244.8" hidden="1">
+    <row r="255" spans="1:20" ht="216" hidden="1">
       <c r="A255" s="20">
         <v>288</v>
       </c>
@@ -16163,7 +16232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="244.8" hidden="1">
+    <row r="256" spans="1:20" ht="288" hidden="1">
       <c r="A256" s="20">
         <v>289</v>
       </c>
@@ -16197,7 +16266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="244.8" hidden="1">
+    <row r="257" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A257" s="20">
         <v>290</v>
       </c>
@@ -16231,7 +16300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="244.8" hidden="1">
+    <row r="258" spans="1:20" ht="158.4" hidden="1">
       <c r="A258" s="20">
         <v>291</v>
       </c>
@@ -16265,7 +16334,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="129.6" hidden="1">
+    <row r="259" spans="1:20" ht="288" hidden="1">
       <c r="A259" s="20">
         <v>292</v>
       </c>
@@ -16299,7 +16368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="259.2" hidden="1">
+    <row r="260" spans="1:20" ht="201.6" hidden="1">
       <c r="A260" s="20">
         <v>293</v>
       </c>
@@ -16333,7 +16402,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="288" hidden="1">
+    <row r="261" spans="1:20" ht="230.4" hidden="1">
       <c r="A261" s="20">
         <v>294</v>
       </c>
@@ -16367,7 +16436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="259.2" hidden="1">
+    <row r="262" spans="1:20" ht="244.8" hidden="1">
       <c r="A262" s="20">
         <v>295</v>
       </c>
@@ -16401,7 +16470,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="216" hidden="1">
+    <row r="263" spans="1:20" ht="244.8" hidden="1">
       <c r="A263" s="20">
         <v>296</v>
       </c>
@@ -16435,7 +16504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="264" spans="1:20" ht="244.8" hidden="1">
       <c r="A264" s="20">
         <v>297</v>
       </c>
@@ -16469,7 +16538,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="288" hidden="1">
+    <row r="265" spans="1:20" ht="244.8" hidden="1">
       <c r="A265" s="20">
         <v>298</v>
       </c>
@@ -16503,7 +16572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="172.8" hidden="1">
+    <row r="266" spans="1:20" ht="244.8" hidden="1">
       <c r="A266" s="20">
         <v>299</v>
       </c>
@@ -16537,7 +16606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="267" spans="1:20" ht="129.6" hidden="1">
       <c r="A267" s="20">
         <v>300</v>
       </c>
@@ -16571,7 +16640,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="201.6" hidden="1">
+    <row r="268" spans="1:20" ht="259.2" hidden="1">
       <c r="A268" s="20">
         <v>301</v>
       </c>
@@ -16605,7 +16674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="230.4" hidden="1">
+    <row r="269" spans="1:20" ht="288" hidden="1">
       <c r="A269" s="20">
         <v>302</v>
       </c>
@@ -16639,7 +16708,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="244.8" hidden="1">
+    <row r="270" spans="1:20" ht="259.2" hidden="1">
       <c r="A270" s="20">
         <v>303</v>
       </c>
@@ -16673,7 +16742,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="244.8" hidden="1">
+    <row r="271" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A271" s="20">
         <v>344</v>
       </c>
@@ -16707,7 +16776,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="244.8" hidden="1">
+    <row r="272" spans="1:20" ht="259.2" hidden="1">
       <c r="A272" s="20">
         <v>345</v>
       </c>
@@ -16741,7 +16810,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="244.8" hidden="1">
+    <row r="273" spans="1:20" ht="230.4" hidden="1">
       <c r="A273" s="20">
         <v>346</v>
       </c>
@@ -16775,7 +16844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="244.8" hidden="1">
+    <row r="274" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A274" s="20">
         <v>347</v>
       </c>
@@ -16809,7 +16878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="129.6" hidden="1">
+    <row r="275" spans="1:20" ht="216" hidden="1">
       <c r="A275" s="20">
         <v>364</v>
       </c>
@@ -16843,7 +16912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="259.2" hidden="1">
+    <row r="276" spans="1:20" ht="244.8" hidden="1">
       <c r="A276" s="20">
         <v>365</v>
       </c>
@@ -16877,7 +16946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="288" hidden="1">
+    <row r="277" spans="1:20" ht="144" hidden="1">
       <c r="A277" s="20">
         <v>20</v>
       </c>
@@ -16911,7 +16980,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="259.2" hidden="1">
+    <row r="278" spans="1:20" ht="144" hidden="1">
       <c r="A278" s="20">
         <v>21</v>
       </c>
@@ -16945,7 +17014,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="216" hidden="1">
+    <row r="279" spans="1:20" ht="144" hidden="1">
       <c r="A279" s="20">
         <v>22</v>
       </c>
@@ -16979,7 +17048,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="288" hidden="1">
+    <row r="280" spans="1:20" ht="144" hidden="1">
       <c r="A280" s="20">
         <v>23</v>
       </c>
@@ -17013,7 +17082,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="281" spans="1:20" ht="144" hidden="1">
       <c r="A281" s="20">
         <v>34</v>
       </c>
@@ -17027,7 +17096,7 @@
         <v>457</v>
       </c>
       <c r="E281" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F281" s="23"/>
       <c r="G281" s="24"/>
@@ -17061,7 +17130,7 @@
         <v>465</v>
       </c>
       <c r="E282" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F282" s="23"/>
       <c r="G282" s="24"/>
@@ -17081,7 +17150,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="288" hidden="1">
+    <row r="283" spans="1:20" ht="43.2" hidden="1">
       <c r="A283" s="20">
         <v>50</v>
       </c>
@@ -17117,7 +17186,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="201.6" hidden="1">
+    <row r="284" spans="1:20" ht="129.6" hidden="1">
       <c r="A284" s="20">
         <v>107</v>
       </c>
@@ -17151,7 +17220,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="230.4" hidden="1">
+    <row r="285" spans="1:20" ht="129.6" hidden="1">
       <c r="A285" s="20">
         <v>108</v>
       </c>
@@ -17185,7 +17254,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="244.8" hidden="1">
+    <row r="286" spans="1:20" ht="129.6" hidden="1">
       <c r="A286" s="20">
         <v>109</v>
       </c>
@@ -17219,7 +17288,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="244.8" hidden="1">
+    <row r="287" spans="1:20" ht="115.2" hidden="1">
       <c r="A287" s="20">
         <v>110</v>
       </c>
@@ -17253,7 +17322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="244.8" hidden="1">
+    <row r="288" spans="1:20" ht="129.6" hidden="1">
       <c r="A288" s="20">
         <v>111</v>
       </c>
@@ -17287,7 +17356,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="244.8" hidden="1">
+    <row r="289" spans="1:20" ht="129.6" hidden="1">
       <c r="A289" s="20">
         <v>112</v>
       </c>
@@ -17321,7 +17390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="244.8" hidden="1">
+    <row r="290" spans="1:20" ht="129.6" hidden="1">
       <c r="A290" s="20">
         <v>113</v>
       </c>
@@ -17389,7 +17458,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="259.2" hidden="1">
+    <row r="292" spans="1:20" ht="129.6" hidden="1">
       <c r="A292" s="20">
         <v>115</v>
       </c>
@@ -17423,7 +17492,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="288" hidden="1">
+    <row r="293" spans="1:20" ht="129.6" hidden="1">
       <c r="A293" s="20">
         <v>116</v>
       </c>
@@ -17457,7 +17526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="259.2" hidden="1">
+    <row r="294" spans="1:20" ht="129.6" hidden="1">
       <c r="A294" s="20">
         <v>117</v>
       </c>
@@ -17491,7 +17560,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="216" hidden="1">
+    <row r="295" spans="1:20" ht="129.6" hidden="1">
       <c r="A295" s="20">
         <v>118</v>
       </c>
@@ -17525,7 +17594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="288" hidden="1">
+    <row r="296" spans="1:20" ht="129.6" hidden="1">
       <c r="A296" s="20">
         <v>119</v>
       </c>
@@ -17559,7 +17628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="297" spans="1:20" ht="129.6" hidden="1">
       <c r="A297" s="20">
         <v>120</v>
       </c>
@@ -17593,7 +17662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="158.4" hidden="1">
+    <row r="298" spans="1:20" ht="129.6" hidden="1">
       <c r="A298" s="20">
         <v>121</v>
       </c>
@@ -17627,7 +17696,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="288" hidden="1">
+    <row r="299" spans="1:20" ht="216" hidden="1">
       <c r="A299" s="20">
         <v>256</v>
       </c>
@@ -17661,7 +17730,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="201.6" hidden="1">
+    <row r="300" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A300" s="20">
         <v>257</v>
       </c>
@@ -17695,7 +17764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="230.4" hidden="1">
+    <row r="301" spans="1:20" ht="288" hidden="1">
       <c r="A301" s="20">
         <v>258</v>
       </c>
@@ -17729,7 +17798,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="244.8" hidden="1">
+    <row r="302" spans="1:20" ht="172.8" hidden="1">
       <c r="A302" s="20">
         <v>259</v>
       </c>
@@ -17763,7 +17832,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="244.8" hidden="1">
+    <row r="303" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A303" s="20">
         <v>260</v>
       </c>
@@ -17797,7 +17866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="244.8" hidden="1">
+    <row r="304" spans="1:20" ht="201.6" hidden="1">
       <c r="A304" s="20">
         <v>261</v>
       </c>
@@ -17831,7 +17900,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="244.8" hidden="1">
+    <row r="305" spans="1:20" ht="230.4" hidden="1">
       <c r="A305" s="20">
         <v>262</v>
       </c>
@@ -17899,7 +17968,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="129.6" hidden="1">
+    <row r="307" spans="1:20" ht="244.8" hidden="1">
       <c r="A307" s="20">
         <v>264</v>
       </c>
@@ -17933,7 +18002,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="259.2" hidden="1">
+    <row r="308" spans="1:20" ht="244.8" hidden="1">
       <c r="A308" s="20">
         <v>265</v>
       </c>
@@ -17967,7 +18036,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="288" hidden="1">
+    <row r="309" spans="1:20" ht="244.8" hidden="1">
       <c r="A309" s="20">
         <v>266</v>
       </c>
@@ -18001,7 +18070,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="259.2" hidden="1">
+    <row r="310" spans="1:20" ht="244.8" hidden="1">
       <c r="A310" s="20">
         <v>267</v>
       </c>
@@ -18035,7 +18104,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="216" hidden="1">
+    <row r="311" spans="1:20" ht="129.6" hidden="1">
       <c r="A311" s="20">
         <v>268</v>
       </c>
@@ -18069,7 +18138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="288" hidden="1">
+    <row r="312" spans="1:20" ht="259.2" hidden="1">
       <c r="A312" s="20">
         <v>269</v>
       </c>
@@ -18103,7 +18172,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="313" spans="1:20" ht="288" hidden="1">
       <c r="A313" s="20">
         <v>270</v>
       </c>
@@ -18137,7 +18206,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="158.4" hidden="1">
+    <row r="314" spans="1:20" ht="259.2" hidden="1">
       <c r="A314" s="20">
         <v>271</v>
       </c>
@@ -18171,7 +18240,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="288" hidden="1">
+    <row r="315" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A315" s="20">
         <v>336</v>
       </c>
@@ -18205,7 +18274,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="201.6" hidden="1">
+    <row r="316" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A316" s="20">
         <v>337</v>
       </c>
@@ -18239,7 +18308,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="230.4" hidden="1">
+    <row r="317" spans="1:20" ht="244.8" hidden="1">
       <c r="A317" s="20">
         <v>338</v>
       </c>
@@ -18273,7 +18342,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="244.8" hidden="1">
+    <row r="318" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A318" s="20">
         <v>339</v>
       </c>
@@ -18307,7 +18376,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="244.8" hidden="1">
+    <row r="319" spans="1:20" ht="216" hidden="1">
       <c r="A319" s="20">
         <v>360</v>
       </c>
@@ -18389,19 +18458,19 @@
         <v>447</v>
       </c>
       <c r="E321" s="22" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="F321" s="23">
         <v>45076</v>
       </c>
       <c r="G321" s="24" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="H321" s="24" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="I321" s="24" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="J321" s="25" t="s">
         <v>776</v>
@@ -18435,19 +18504,19 @@
         <v>448</v>
       </c>
       <c r="E322" s="22" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="F322" s="23">
         <v>45076</v>
       </c>
       <c r="G322" s="24" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="H322" s="24" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="I322" s="24" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="J322" s="25" t="s">
         <v>776</v>
@@ -18481,19 +18550,19 @@
         <v>449</v>
       </c>
       <c r="E323" s="22" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="F323" s="23">
         <v>45076</v>
       </c>
       <c r="G323" s="24" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="H323" s="24" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="I323" s="24" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="J323" s="25" t="s">
         <v>776</v>
@@ -18527,19 +18596,19 @@
         <v>450</v>
       </c>
       <c r="E324" s="22" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="F324" s="23">
         <v>45076</v>
       </c>
       <c r="G324" s="24" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="H324" s="24" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="I324" s="24" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="J324" s="25" t="s">
         <v>776</v>
@@ -18573,16 +18642,16 @@
         <v>458</v>
       </c>
       <c r="E325" s="22" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F325" s="23">
         <v>45076</v>
       </c>
       <c r="G325" s="24" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="H325" s="24" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="I325" s="24" t="s">
         <v>775</v>
@@ -18598,13 +18667,13 @@
         <v>469</v>
       </c>
       <c r="N325" s="25" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O325" s="25" t="s">
-        <v>774</v>
+        <v>469</v>
       </c>
       <c r="P325" s="25" t="s">
-        <v>777</v>
+        <v>972</v>
       </c>
       <c r="Q325" s="25" t="s">
         <v>772</v>
@@ -18629,16 +18698,16 @@
         <v>466</v>
       </c>
       <c r="E326" s="22" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F326" s="23">
         <v>45076</v>
       </c>
       <c r="G326" s="24" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="H326" s="24" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="I326" s="24" t="s">
         <v>775</v>
@@ -18654,13 +18723,13 @@
         <v>469</v>
       </c>
       <c r="N326" s="25" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O326" s="25" t="s">
-        <v>774</v>
-      </c>
-      <c r="P326" s="25" t="s">
-        <v>777</v>
+        <v>469</v>
+      </c>
+      <c r="P326" s="46" t="s">
+        <v>966</v>
       </c>
       <c r="Q326" s="25" t="s">
         <v>772</v>
@@ -18702,13 +18771,13 @@
         <v>469</v>
       </c>
       <c r="N327" s="25" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="O327" s="25" t="s">
-        <v>774</v>
-      </c>
-      <c r="P327" s="25" t="s">
-        <v>782</v>
+        <v>469</v>
+      </c>
+      <c r="P327" s="46" t="s">
+        <v>965</v>
       </c>
       <c r="Q327" s="25" t="s">
         <v>772</v>
@@ -18721,59 +18790,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="115.2">
-      <c r="A328" s="20">
+    <row r="328" spans="1:20" s="55" customFormat="1" ht="115.2">
+      <c r="A328" s="47">
         <v>122</v>
       </c>
-      <c r="B328" s="21" t="s">
+      <c r="B328" s="45" t="s">
         <v>404</v>
       </c>
-      <c r="C328" s="21" t="s">
+      <c r="C328" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D328" s="21" t="s">
+      <c r="D328" s="48" t="s">
         <v>607</v>
       </c>
-      <c r="E328" s="22" t="s">
-        <v>941</v>
-      </c>
-      <c r="F328" s="23">
+      <c r="E328" s="49" t="s">
+        <v>938</v>
+      </c>
+      <c r="F328" s="50">
         <v>45076</v>
       </c>
-      <c r="G328" s="24" t="s">
-        <v>802</v>
-      </c>
-      <c r="H328" s="24" t="s">
-        <v>803</v>
-      </c>
-      <c r="I328" s="24" t="s">
-        <v>804</v>
-      </c>
-      <c r="J328" s="25" t="s">
+      <c r="G328" s="51" t="s">
+        <v>799</v>
+      </c>
+      <c r="H328" s="51" t="s">
+        <v>800</v>
+      </c>
+      <c r="I328" s="51" t="s">
+        <v>801</v>
+      </c>
+      <c r="J328" s="46" t="s">
         <v>776</v>
       </c>
-      <c r="K328" s="25"/>
-      <c r="L328" s="25" t="s">
+      <c r="K328" s="46"/>
+      <c r="L328" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="M328" s="25" t="s">
+      <c r="M328" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="N328" s="25" t="s">
-        <v>780</v>
-      </c>
-      <c r="O328" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P328" s="25" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q328" s="25" t="s">
+      <c r="N328" s="46" t="s">
+        <v>779</v>
+      </c>
+      <c r="O328" s="46" t="s">
+        <v>774</v>
+      </c>
+      <c r="P328" s="46" t="s">
+        <v>969</v>
+      </c>
+      <c r="Q328" s="46" t="s">
         <v>772</v>
       </c>
-      <c r="R328" s="26"/>
-      <c r="S328" s="27"/>
-      <c r="T328" s="28" t="s">
+      <c r="R328" s="52"/>
+      <c r="S328" s="53"/>
+      <c r="T328" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -18791,16 +18860,16 @@
         <v>608</v>
       </c>
       <c r="E329" s="22" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="F329" s="23">
         <v>45076</v>
       </c>
       <c r="G329" s="24" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="H329" s="24" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="I329" s="24" t="s">
         <v>775</v>
@@ -18816,13 +18885,13 @@
         <v>469</v>
       </c>
       <c r="N329" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O329" s="25" t="s">
-        <v>469</v>
+        <v>774</v>
       </c>
       <c r="P329" s="25" t="s">
-        <v>781</v>
+        <v>970</v>
       </c>
       <c r="Q329" s="25" t="s">
         <v>772</v>
@@ -18833,59 +18902,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="115.2">
-      <c r="A330" s="20">
+    <row r="330" spans="1:20" s="55" customFormat="1" ht="115.2">
+      <c r="A330" s="47">
         <v>124</v>
       </c>
-      <c r="B330" s="21" t="s">
+      <c r="B330" s="45" t="s">
         <v>404</v>
       </c>
-      <c r="C330" s="21" t="s">
+      <c r="C330" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D330" s="21" t="s">
+      <c r="D330" s="48" t="s">
         <v>609</v>
       </c>
-      <c r="E330" s="22" t="s">
-        <v>943</v>
-      </c>
-      <c r="F330" s="23">
+      <c r="E330" s="49" t="s">
+        <v>940</v>
+      </c>
+      <c r="F330" s="50">
         <v>45076</v>
       </c>
-      <c r="G330" s="24" t="s">
-        <v>807</v>
-      </c>
-      <c r="H330" s="24" t="s">
-        <v>808</v>
-      </c>
-      <c r="I330" s="24" t="s">
-        <v>809</v>
-      </c>
-      <c r="J330" s="25" t="s">
+      <c r="G330" s="51" t="s">
+        <v>804</v>
+      </c>
+      <c r="H330" s="51" t="s">
+        <v>805</v>
+      </c>
+      <c r="I330" s="51" t="s">
+        <v>806</v>
+      </c>
+      <c r="J330" s="46" t="s">
         <v>776</v>
       </c>
-      <c r="K330" s="25"/>
-      <c r="L330" s="25" t="s">
+      <c r="K330" s="46"/>
+      <c r="L330" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="M330" s="25" t="s">
+      <c r="M330" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="N330" s="25" t="s">
-        <v>780</v>
-      </c>
-      <c r="O330" s="25" t="s">
+      <c r="N330" s="46" t="s">
+        <v>779</v>
+      </c>
+      <c r="O330" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="P330" s="25" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q330" s="25" t="s">
+      <c r="P330" s="46" t="s">
+        <v>967</v>
+      </c>
+      <c r="Q330" s="46" t="s">
         <v>772</v>
       </c>
-      <c r="R330" s="26"/>
-      <c r="S330" s="27"/>
-      <c r="T330" s="28" t="s">
+      <c r="R330" s="52"/>
+      <c r="S330" s="53"/>
+      <c r="T330" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -18903,19 +18972,19 @@
         <v>610</v>
       </c>
       <c r="E331" s="22" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="F331" s="23">
         <v>45076</v>
       </c>
       <c r="G331" s="24" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="H331" s="24" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="I331" s="24" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="J331" s="25" t="s">
         <v>776</v>
@@ -18928,13 +18997,13 @@
         <v>469</v>
       </c>
       <c r="N331" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O331" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P331" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P331" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q331" s="25" t="s">
         <v>772</v>
@@ -18959,19 +19028,19 @@
         <v>611</v>
       </c>
       <c r="E332" s="22" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="F332" s="23">
         <v>45076</v>
       </c>
       <c r="G332" s="24" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="H332" s="24" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="I332" s="24" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="J332" s="25" t="s">
         <v>776</v>
@@ -18984,13 +19053,13 @@
         <v>469</v>
       </c>
       <c r="N332" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O332" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P332" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P332" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q332" s="25" t="s">
         <v>772</v>
@@ -19015,19 +19084,19 @@
         <v>612</v>
       </c>
       <c r="E333" s="22" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="F333" s="23">
         <v>45076</v>
       </c>
       <c r="G333" s="24" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="H333" s="24" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="I333" s="24" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="J333" s="25" t="s">
         <v>776</v>
@@ -19040,13 +19109,13 @@
         <v>469</v>
       </c>
       <c r="N333" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O333" s="25" t="s">
-        <v>469</v>
+        <v>774</v>
       </c>
       <c r="P333" s="25" t="s">
-        <v>781</v>
+        <v>970</v>
       </c>
       <c r="Q333" s="25" t="s">
         <v>772</v>
@@ -19071,19 +19140,19 @@
         <v>613</v>
       </c>
       <c r="E334" s="22" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="F334" s="23">
         <v>45076</v>
       </c>
       <c r="G334" s="24" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="H334" s="24" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="I334" s="24" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="J334" s="25" t="s">
         <v>776</v>
@@ -19096,13 +19165,13 @@
         <v>469</v>
       </c>
       <c r="N334" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O334" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P334" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P334" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q334" s="25" t="s">
         <v>772</v>
@@ -19127,19 +19196,19 @@
         <v>614</v>
       </c>
       <c r="E335" s="22" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="F335" s="23">
         <v>45076</v>
       </c>
       <c r="G335" s="24" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="H335" s="24" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="I335" s="24" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="J335" s="25" t="s">
         <v>776</v>
@@ -19152,13 +19221,13 @@
         <v>469</v>
       </c>
       <c r="N335" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O335" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P335" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P335" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q335" s="25" t="s">
         <v>772</v>
@@ -19183,19 +19252,19 @@
         <v>615</v>
       </c>
       <c r="E336" s="22" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="F336" s="23">
         <v>45076</v>
       </c>
       <c r="G336" s="24" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="H336" s="24" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I336" s="24" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="J336" s="25" t="s">
         <v>776</v>
@@ -19208,13 +19277,13 @@
         <v>469</v>
       </c>
       <c r="N336" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O336" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P336" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P336" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q336" s="25" t="s">
         <v>772</v>
@@ -19239,19 +19308,19 @@
         <v>616</v>
       </c>
       <c r="E337" s="22" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="F337" s="23">
         <v>45076</v>
       </c>
       <c r="G337" s="24" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="H337" s="24" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="I337" s="24" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="J337" s="25" t="s">
         <v>776</v>
@@ -19264,13 +19333,13 @@
         <v>469</v>
       </c>
       <c r="N337" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O337" s="25" t="s">
-        <v>469</v>
+        <v>774</v>
       </c>
       <c r="P337" s="25" t="s">
-        <v>781</v>
+        <v>970</v>
       </c>
       <c r="Q337" s="25" t="s">
         <v>772</v>
@@ -19295,19 +19364,19 @@
         <v>617</v>
       </c>
       <c r="E338" s="22" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="F338" s="23">
         <v>45076</v>
       </c>
       <c r="G338" s="24" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="H338" s="24" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="I338" s="24" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="J338" s="25" t="s">
         <v>776</v>
@@ -19320,13 +19389,13 @@
         <v>469</v>
       </c>
       <c r="N338" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O338" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P338" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P338" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q338" s="25" t="s">
         <v>772</v>
@@ -19351,19 +19420,19 @@
         <v>618</v>
       </c>
       <c r="E339" s="22" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="F339" s="23">
         <v>45076</v>
       </c>
       <c r="G339" s="24" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="H339" s="24" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="I339" s="24" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="J339" s="25" t="s">
         <v>776</v>
@@ -19376,13 +19445,13 @@
         <v>469</v>
       </c>
       <c r="N339" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O339" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P339" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P339" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q339" s="25" t="s">
         <v>772</v>
@@ -19407,19 +19476,19 @@
         <v>619</v>
       </c>
       <c r="E340" s="22" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="F340" s="23">
         <v>45076</v>
       </c>
       <c r="G340" s="24" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="H340" s="24" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="I340" s="24" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="J340" s="25" t="s">
         <v>776</v>
@@ -19432,13 +19501,13 @@
         <v>469</v>
       </c>
       <c r="N340" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O340" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P340" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P340" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q340" s="25" t="s">
         <v>772</v>
@@ -19463,19 +19532,19 @@
         <v>620</v>
       </c>
       <c r="E341" s="22" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="F341" s="23">
         <v>45076</v>
       </c>
       <c r="G341" s="24" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="H341" s="24" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I341" s="24" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="J341" s="25" t="s">
         <v>776</v>
@@ -19488,13 +19557,13 @@
         <v>469</v>
       </c>
       <c r="N341" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O341" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P341" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P341" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q341" s="25" t="s">
         <v>772</v>
@@ -19519,19 +19588,19 @@
         <v>621</v>
       </c>
       <c r="E342" s="22" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="F342" s="23">
         <v>45076</v>
       </c>
       <c r="G342" s="24" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="H342" s="24" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="I342" s="24" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="J342" s="25" t="s">
         <v>776</v>
@@ -19544,13 +19613,13 @@
         <v>469</v>
       </c>
       <c r="N342" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O342" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P342" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P342" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q342" s="25" t="s">
         <v>772</v>
@@ -19575,19 +19644,19 @@
         <v>622</v>
       </c>
       <c r="E343" s="22" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="F343" s="23">
         <v>45076</v>
       </c>
       <c r="G343" s="24" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="H343" s="24" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="I343" s="24" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J343" s="25" t="s">
         <v>776</v>
@@ -19600,13 +19669,13 @@
         <v>469</v>
       </c>
       <c r="N343" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O343" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P343" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P343" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q343" s="25" t="s">
         <v>772</v>
@@ -19631,19 +19700,19 @@
         <v>623</v>
       </c>
       <c r="E344" s="22" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="F344" s="23">
         <v>45076</v>
       </c>
       <c r="G344" s="24" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="H344" s="24" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="I344" s="24" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="J344" s="25" t="s">
         <v>776</v>
@@ -19656,13 +19725,13 @@
         <v>469</v>
       </c>
       <c r="N344" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O344" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P344" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P344" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q344" s="25" t="s">
         <v>772</v>
@@ -19687,19 +19756,19 @@
         <v>624</v>
       </c>
       <c r="E345" s="22" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="F345" s="23">
         <v>45076</v>
       </c>
       <c r="G345" s="24" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="H345" s="24" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="I345" s="24" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="J345" s="25" t="s">
         <v>776</v>
@@ -19712,13 +19781,13 @@
         <v>469</v>
       </c>
       <c r="N345" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O345" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P345" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P345" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q345" s="25" t="s">
         <v>772</v>
@@ -19743,19 +19812,19 @@
         <v>625</v>
       </c>
       <c r="E346" s="22" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="F346" s="23">
         <v>45076</v>
       </c>
       <c r="G346" s="24" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="H346" s="24" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="I346" s="24" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="J346" s="25" t="s">
         <v>776</v>
@@ -19768,13 +19837,13 @@
         <v>469</v>
       </c>
       <c r="N346" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O346" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P346" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P346" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q346" s="25" t="s">
         <v>772</v>
@@ -19799,19 +19868,19 @@
         <v>626</v>
       </c>
       <c r="E347" s="22" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="F347" s="23">
         <v>45076</v>
       </c>
       <c r="G347" s="24" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="H347" s="24" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="I347" s="24" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="J347" s="25" t="s">
         <v>776</v>
@@ -19824,13 +19893,13 @@
         <v>469</v>
       </c>
       <c r="N347" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O347" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P347" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P347" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q347" s="25" t="s">
         <v>772</v>
@@ -19855,19 +19924,19 @@
         <v>627</v>
       </c>
       <c r="E348" s="22" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="F348" s="23">
         <v>45076</v>
       </c>
       <c r="G348" s="24" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="H348" s="24" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="I348" s="24" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="J348" s="25" t="s">
         <v>776</v>
@@ -19880,13 +19949,13 @@
         <v>469</v>
       </c>
       <c r="N348" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O348" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P348" s="25" t="s">
-        <v>781</v>
+        <v>968</v>
       </c>
       <c r="Q348" s="25" t="s">
         <v>772</v>
@@ -19911,19 +19980,19 @@
         <v>628</v>
       </c>
       <c r="E349" s="22" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="F349" s="23">
         <v>45076</v>
       </c>
       <c r="G349" s="24" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="H349" s="24" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="I349" s="24" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="J349" s="25" t="s">
         <v>776</v>
@@ -19936,13 +20005,13 @@
         <v>469</v>
       </c>
       <c r="N349" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O349" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P349" s="25" t="s">
-        <v>781</v>
+        <v>968</v>
       </c>
       <c r="Q349" s="25" t="s">
         <v>772</v>
@@ -19967,19 +20036,19 @@
         <v>629</v>
       </c>
       <c r="E350" s="22" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="F350" s="23">
         <v>45076</v>
       </c>
       <c r="G350" s="24" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="H350" s="24" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="I350" s="24" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="J350" s="25" t="s">
         <v>776</v>
@@ -19992,13 +20061,13 @@
         <v>469</v>
       </c>
       <c r="N350" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O350" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P350" s="25" t="s">
-        <v>781</v>
+        <v>968</v>
       </c>
       <c r="Q350" s="25" t="s">
         <v>772</v>
@@ -20023,19 +20092,19 @@
         <v>630</v>
       </c>
       <c r="E351" s="22" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="F351" s="23">
         <v>45076</v>
       </c>
       <c r="G351" s="24" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="H351" s="24" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="I351" s="24" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="J351" s="25" t="s">
         <v>776</v>
@@ -20048,13 +20117,13 @@
         <v>469</v>
       </c>
       <c r="N351" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O351" s="25" t="s">
         <v>469</v>
       </c>
       <c r="P351" s="25" t="s">
-        <v>781</v>
+        <v>968</v>
       </c>
       <c r="Q351" s="25" t="s">
         <v>772</v>
@@ -20079,19 +20148,19 @@
         <v>631</v>
       </c>
       <c r="E352" s="22" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F352" s="23">
         <v>45076</v>
       </c>
       <c r="G352" s="24" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="H352" s="24" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="I352" s="24" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="J352" s="25" t="s">
         <v>776</v>
@@ -20104,13 +20173,13 @@
         <v>469</v>
       </c>
       <c r="N352" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="O352" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="P352" s="25" t="s">
-        <v>781</v>
+        <v>774</v>
+      </c>
+      <c r="P352" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="Q352" s="25" t="s">
         <v>772</v>
@@ -20121,7 +20190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="230.4" hidden="1">
+    <row r="353" spans="1:20" ht="216" hidden="1">
       <c r="A353" s="20">
         <v>272</v>
       </c>
@@ -20155,7 +20224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="354" spans="1:20" ht="288" hidden="1">
       <c r="A354" s="20">
         <v>273</v>
       </c>
@@ -20189,7 +20258,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="302.39999999999998" hidden="1">
+    <row r="355" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A355" s="20">
         <v>274</v>
       </c>
@@ -20223,7 +20292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="356" spans="1:20" ht="158.4" hidden="1">
       <c r="A356" s="20">
         <v>275</v>
       </c>
@@ -20257,7 +20326,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="244.8" hidden="1">
+    <row r="357" spans="1:20" ht="288" hidden="1">
       <c r="A357" s="20">
         <v>276</v>
       </c>
@@ -20291,7 +20360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="273.60000000000002" hidden="1">
+    <row r="358" spans="1:20" ht="201.6" hidden="1">
       <c r="A358" s="20">
         <v>277</v>
       </c>
@@ -20325,7 +20394,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="216" hidden="1">
+    <row r="359" spans="1:20" ht="230.4" hidden="1">
       <c r="A359" s="20">
         <v>278</v>
       </c>
@@ -20393,7 +20462,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="216" hidden="1">
+    <row r="361" spans="1:20" ht="244.8" hidden="1">
       <c r="A361" s="20">
         <v>280</v>
       </c>
@@ -20461,7 +20530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="216" hidden="1">
+    <row r="363" spans="1:20" ht="244.8" hidden="1">
       <c r="A363" s="20">
         <v>282</v>
       </c>
@@ -20529,7 +20598,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="216" hidden="1">
+    <row r="365" spans="1:20" ht="129.6" hidden="1">
       <c r="A365" s="20">
         <v>284</v>
       </c>
@@ -20563,7 +20632,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="244.8" hidden="1">
+    <row r="366" spans="1:20" ht="259.2" hidden="1">
       <c r="A366" s="20">
         <v>285</v>
       </c>
@@ -20597,7 +20666,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="216" hidden="1">
+    <row r="367" spans="1:20" ht="288" hidden="1">
       <c r="A367" s="20">
         <v>286</v>
       </c>
@@ -20631,7 +20700,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="244.8" hidden="1">
+    <row r="368" spans="1:20" ht="259.2" hidden="1">
       <c r="A368" s="20">
         <v>287</v>
       </c>
@@ -20665,7 +20734,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="216" hidden="1">
+    <row r="369" spans="1:20" ht="302.39999999999998" hidden="1">
       <c r="A369" s="20">
         <v>340</v>
       </c>
@@ -20699,7 +20768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="244.8" hidden="1">
+    <row r="370" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A370" s="20">
         <v>341</v>
       </c>
@@ -20733,7 +20802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="216" hidden="1">
+    <row r="371" spans="1:20" ht="244.8" hidden="1">
       <c r="A371" s="20">
         <v>342</v>
       </c>
@@ -20767,7 +20836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="244.8" hidden="1">
+    <row r="372" spans="1:20" ht="273.60000000000002" hidden="1">
       <c r="A372" s="20">
         <v>343</v>
       </c>

</xml_diff>

<commit_message>
aggiunte valore su colonne mancanti
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
+++ b/GATEWAY/S1#111PRAEZISIONX/PRAEZISION/ISOLABELLA/3.29.0.X/report_checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://praezisionsrl-my.sharepoint.com/personal/motilli_praezisionsrl_onmicrosoft_com/Documents/Progetti/FSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\AzurePRZ\FSE-ACCREDITAMENTO\GATEWAY\S1#111PRAEZISIONX\PRAEZISION\ISOLABELLA\3.29.0.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{65C7D956-A811-4651-94F3-61F4578CC891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17A0FF57-F4E7-493C-A2AE-41964D6A2C75}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4D59D2-D4F1-4D05-9F66-DCF3A8D41492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="806">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -5264,13 +5264,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B166" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5560,7 +5561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -5595,7 +5596,7 @@
       <c r="V10" s="36"/>
       <c r="W10" s="37"/>
     </row>
-    <row r="11" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>2</v>
       </c>
@@ -5630,7 +5631,7 @@
       <c r="V11" s="36"/>
       <c r="W11" s="37"/>
     </row>
-    <row r="12" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>3</v>
       </c>
@@ -5665,7 +5666,7 @@
       <c r="V12" s="36"/>
       <c r="W12" s="37"/>
     </row>
-    <row r="13" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>4</v>
       </c>
@@ -5700,7 +5701,7 @@
       <c r="V13" s="36"/>
       <c r="W13" s="37"/>
     </row>
-    <row r="14" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>5</v>
       </c>
@@ -5931,7 +5932,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -5966,7 +5967,7 @@
       <c r="V19" s="36"/>
       <c r="W19" s="37"/>
     </row>
-    <row r="20" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -6001,7 +6002,7 @@
       <c r="V20" s="36"/>
       <c r="W20" s="37"/>
     </row>
-    <row r="21" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -6036,7 +6037,7 @@
       <c r="V21" s="36"/>
       <c r="W21" s="37"/>
     </row>
-    <row r="22" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -6071,7 +6072,7 @@
       <c r="V22" s="36"/>
       <c r="W22" s="37"/>
     </row>
-    <row r="23" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -6106,7 +6107,7 @@
       <c r="V23" s="36"/>
       <c r="W23" s="37"/>
     </row>
-    <row r="24" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
         <v>21</v>
       </c>
@@ -6141,7 +6142,7 @@
       <c r="V24" s="36"/>
       <c r="W24" s="37"/>
     </row>
-    <row r="25" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29">
         <v>22</v>
       </c>
@@ -6176,7 +6177,7 @@
       <c r="V25" s="36"/>
       <c r="W25" s="37"/>
     </row>
-    <row r="26" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
         <v>23</v>
       </c>
@@ -6407,7 +6408,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
         <v>28</v>
       </c>
@@ -6487,8 +6488,12 @@
       <c r="P32" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
+      <c r="Q32" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R32" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S32" s="69" t="s">
         <v>796</v>
       </c>
@@ -6501,7 +6506,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="29">
         <v>30</v>
       </c>
@@ -6581,8 +6586,12 @@
       <c r="P34" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
+      <c r="Q34" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R34" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S34" s="69" t="s">
         <v>797</v>
       </c>
@@ -6640,8 +6649,12 @@
       <c r="P35" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
+      <c r="Q35" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R35" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S35" s="69" t="s">
         <v>797</v>
       </c>
@@ -6654,7 +6667,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
         <v>33</v>
       </c>
@@ -6689,7 +6702,7 @@
       <c r="V36" s="36"/>
       <c r="W36" s="37"/>
     </row>
-    <row r="37" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
         <v>34</v>
       </c>
@@ -6769,8 +6782,12 @@
       <c r="P38" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
+      <c r="Q38" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R38" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S38" s="69" t="s">
         <v>796</v>
       </c>
@@ -6783,7 +6800,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
         <v>36</v>
       </c>
@@ -6863,8 +6880,12 @@
       <c r="P40" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
+      <c r="Q40" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R40" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S40" s="69" t="s">
         <v>797</v>
       </c>
@@ -6877,7 +6898,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
         <v>38</v>
       </c>
@@ -6957,8 +6978,12 @@
       <c r="P42" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q42" s="34"/>
-      <c r="R42" s="34"/>
+      <c r="Q42" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R42" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S42" s="69" t="s">
         <v>797</v>
       </c>
@@ -7016,8 +7041,12 @@
       <c r="P43" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q43" s="34"/>
-      <c r="R43" s="34"/>
+      <c r="Q43" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R43" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S43" s="69" t="s">
         <v>797</v>
       </c>
@@ -7030,7 +7059,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
         <v>41</v>
       </c>
@@ -7065,7 +7094,7 @@
       <c r="V44" s="36"/>
       <c r="W44" s="37"/>
     </row>
-    <row r="45" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="29">
         <v>42</v>
       </c>
@@ -7145,8 +7174,12 @@
       <c r="P46" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
+      <c r="Q46" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R46" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S46" s="69" t="s">
         <v>797</v>
       </c>
@@ -7159,7 +7192,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="29">
         <v>44</v>
       </c>
@@ -7233,8 +7266,12 @@
       <c r="P48" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
+      <c r="Q48" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R48" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S48" s="69" t="s">
         <v>799</v>
       </c>
@@ -7249,7 +7286,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>46</v>
       </c>
@@ -7323,8 +7360,12 @@
       <c r="P50" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q50" s="34"/>
-      <c r="R50" s="34"/>
+      <c r="Q50" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R50" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S50" s="69" t="s">
         <v>799</v>
       </c>
@@ -7378,8 +7419,12 @@
       <c r="P51" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="34"/>
+      <c r="Q51" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R51" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S51" s="69" t="s">
         <v>799</v>
       </c>
@@ -7394,7 +7439,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="29">
         <v>49</v>
       </c>
@@ -7429,7 +7474,7 @@
       <c r="V52" s="36"/>
       <c r="W52" s="37"/>
     </row>
-    <row r="53" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="29">
         <v>50</v>
       </c>
@@ -7503,8 +7548,12 @@
       <c r="P54" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
+      <c r="Q54" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R54" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S54" s="69" t="s">
         <v>799</v>
       </c>
@@ -7519,7 +7568,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="29">
         <v>52</v>
       </c>
@@ -7554,7 +7603,7 @@
       <c r="V55" s="36"/>
       <c r="W55" s="37"/>
     </row>
-    <row r="56" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>53</v>
       </c>
@@ -7589,7 +7638,7 @@
       <c r="V56" s="36"/>
       <c r="W56" s="37"/>
     </row>
-    <row r="57" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="29">
         <v>54</v>
       </c>
@@ -7624,7 +7673,7 @@
       <c r="V57" s="36"/>
       <c r="W57" s="37"/>
     </row>
-    <row r="58" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="29">
         <v>55</v>
       </c>
@@ -7659,7 +7708,7 @@
       <c r="V58" s="36"/>
       <c r="W58" s="37"/>
     </row>
-    <row r="59" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="29">
         <v>56</v>
       </c>
@@ -7694,7 +7743,7 @@
       <c r="V59" s="36"/>
       <c r="W59" s="37"/>
     </row>
-    <row r="60" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="29">
         <v>57</v>
       </c>
@@ -7729,7 +7778,7 @@
       <c r="V60" s="36"/>
       <c r="W60" s="37"/>
     </row>
-    <row r="61" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="29">
         <v>58</v>
       </c>
@@ -7764,7 +7813,7 @@
       <c r="V61" s="36"/>
       <c r="W61" s="37"/>
     </row>
-    <row r="62" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="29">
         <v>59</v>
       </c>
@@ -7799,7 +7848,7 @@
       <c r="V62" s="36"/>
       <c r="W62" s="37"/>
     </row>
-    <row r="63" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="29">
         <v>60</v>
       </c>
@@ -7834,7 +7883,7 @@
       <c r="V63" s="36"/>
       <c r="W63" s="37"/>
     </row>
-    <row r="64" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="29">
         <v>61</v>
       </c>
@@ -7869,7 +7918,7 @@
       <c r="V64" s="36"/>
       <c r="W64" s="37"/>
     </row>
-    <row r="65" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="29">
         <v>62</v>
       </c>
@@ -7949,8 +7998,12 @@
       <c r="P66" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q66" s="34"/>
-      <c r="R66" s="34"/>
+      <c r="Q66" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R66" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S66" s="69" t="s">
         <v>801</v>
       </c>
@@ -8008,8 +8061,12 @@
       <c r="P67" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q67" s="34"/>
-      <c r="R67" s="34"/>
+      <c r="Q67" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R67" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S67" s="69" t="s">
         <v>802</v>
       </c>
@@ -8067,8 +8124,12 @@
       <c r="P68" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q68" s="34"/>
-      <c r="R68" s="34"/>
+      <c r="Q68" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R68" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S68" s="69" t="s">
         <v>803</v>
       </c>
@@ -8126,8 +8187,12 @@
       <c r="P69" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q69" s="34"/>
-      <c r="R69" s="34"/>
+      <c r="Q69" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R69" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S69" s="69" t="s">
         <v>801</v>
       </c>
@@ -8185,8 +8250,12 @@
       <c r="P70" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
+      <c r="Q70" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R70" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S70" s="69" t="s">
         <v>801</v>
       </c>
@@ -8244,8 +8313,12 @@
       <c r="P71" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q71" s="34"/>
-      <c r="R71" s="34"/>
+      <c r="Q71" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R71" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S71" s="69" t="s">
         <v>802</v>
       </c>
@@ -8303,8 +8376,12 @@
       <c r="P72" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q72" s="34"/>
-      <c r="R72" s="34"/>
+      <c r="Q72" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R72" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S72" s="69" t="s">
         <v>801</v>
       </c>
@@ -8362,8 +8439,12 @@
       <c r="P73" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q73" s="34"/>
-      <c r="R73" s="34"/>
+      <c r="Q73" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R73" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S73" s="69" t="s">
         <v>801</v>
       </c>
@@ -8421,8 +8502,12 @@
       <c r="P74" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q74" s="34"/>
-      <c r="R74" s="34"/>
+      <c r="Q74" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R74" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S74" s="69" t="s">
         <v>801</v>
       </c>
@@ -8480,8 +8565,12 @@
       <c r="P75" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q75" s="34"/>
-      <c r="R75" s="34"/>
+      <c r="Q75" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R75" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S75" s="69" t="s">
         <v>801</v>
       </c>
@@ -8539,8 +8628,12 @@
       <c r="P76" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q76" s="34"/>
-      <c r="R76" s="34"/>
+      <c r="Q76" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R76" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S76" s="69" t="s">
         <v>804</v>
       </c>
@@ -8598,8 +8691,12 @@
       <c r="P77" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q77" s="34"/>
-      <c r="R77" s="34"/>
+      <c r="Q77" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R77" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S77" s="69" t="s">
         <v>804</v>
       </c>
@@ -8657,8 +8754,12 @@
       <c r="P78" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q78" s="34"/>
-      <c r="R78" s="34"/>
+      <c r="Q78" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R78" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S78" s="70" t="s">
         <v>801</v>
       </c>
@@ -8716,8 +8817,12 @@
       <c r="P79" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q79" s="34"/>
-      <c r="R79" s="34"/>
+      <c r="Q79" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R79" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S79" s="34" t="s">
         <v>802</v>
       </c>
@@ -8775,8 +8880,12 @@
       <c r="P80" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q80" s="34"/>
-      <c r="R80" s="34"/>
+      <c r="Q80" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R80" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S80" s="34" t="s">
         <v>802</v>
       </c>
@@ -8834,8 +8943,12 @@
       <c r="P81" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="Q81" s="34"/>
-      <c r="R81" s="34"/>
+      <c r="Q81" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R81" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S81" s="34" t="s">
         <v>802</v>
       </c>
@@ -8893,8 +9006,12 @@
       <c r="P82" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q82" s="34"/>
-      <c r="R82" s="34"/>
+      <c r="Q82" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R82" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S82" s="34" t="s">
         <v>801</v>
       </c>
@@ -8952,8 +9069,12 @@
       <c r="P83" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q83" s="34"/>
-      <c r="R83" s="34"/>
+      <c r="Q83" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R83" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S83" s="34" t="s">
         <v>802</v>
       </c>
@@ -9011,8 +9132,12 @@
       <c r="P84" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q84" s="34"/>
-      <c r="R84" s="34"/>
+      <c r="Q84" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R84" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S84" s="34" t="s">
         <v>801</v>
       </c>
@@ -9070,8 +9195,12 @@
       <c r="P85" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q85" s="34"/>
-      <c r="R85" s="34"/>
+      <c r="Q85" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R85" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S85" s="34" t="s">
         <v>802</v>
       </c>
@@ -9129,8 +9258,12 @@
       <c r="P86" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q86" s="34"/>
-      <c r="R86" s="34"/>
+      <c r="Q86" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R86" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S86" s="34" t="s">
         <v>801</v>
       </c>
@@ -9188,8 +9321,12 @@
       <c r="P87" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q87" s="34"/>
-      <c r="R87" s="34"/>
+      <c r="Q87" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R87" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S87" s="34" t="s">
         <v>801</v>
       </c>
@@ -9247,8 +9384,12 @@
       <c r="P88" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q88" s="34"/>
-      <c r="R88" s="34"/>
+      <c r="Q88" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R88" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S88" s="34" t="s">
         <v>801</v>
       </c>
@@ -9306,8 +9447,12 @@
       <c r="P89" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q89" s="34"/>
-      <c r="R89" s="34"/>
+      <c r="Q89" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R89" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S89" s="34" t="s">
         <v>801</v>
       </c>
@@ -9365,8 +9510,12 @@
       <c r="P90" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q90" s="34"/>
-      <c r="R90" s="34"/>
+      <c r="Q90" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R90" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S90" s="34" t="s">
         <v>801</v>
       </c>
@@ -9424,8 +9573,12 @@
       <c r="P91" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q91" s="34"/>
-      <c r="R91" s="34"/>
+      <c r="Q91" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R91" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S91" s="34" t="s">
         <v>801</v>
       </c>
@@ -9483,8 +9636,12 @@
       <c r="P92" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q92" s="34"/>
-      <c r="R92" s="34"/>
+      <c r="Q92" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R92" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S92" s="34" t="s">
         <v>801</v>
       </c>
@@ -9542,8 +9699,12 @@
       <c r="P93" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q93" s="34"/>
-      <c r="R93" s="34"/>
+      <c r="Q93" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R93" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S93" s="34" t="s">
         <v>801</v>
       </c>
@@ -9601,8 +9762,12 @@
       <c r="P94" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q94" s="34"/>
-      <c r="R94" s="34"/>
+      <c r="Q94" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R94" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S94" s="34" t="s">
         <v>801</v>
       </c>
@@ -9660,8 +9825,12 @@
       <c r="P95" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q95" s="34"/>
-      <c r="R95" s="34"/>
+      <c r="Q95" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R95" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S95" s="34" t="s">
         <v>801</v>
       </c>
@@ -9719,8 +9888,12 @@
       <c r="P96" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q96" s="34"/>
-      <c r="R96" s="34"/>
+      <c r="Q96" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R96" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S96" s="34" t="s">
         <v>801</v>
       </c>
@@ -9733,7 +9906,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="29">
         <v>94</v>
       </c>
@@ -9768,7 +9941,7 @@
       <c r="V97" s="36"/>
       <c r="W97" s="37"/>
     </row>
-    <row r="98" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="29">
         <v>95</v>
       </c>
@@ -9803,7 +9976,7 @@
       <c r="V98" s="36"/>
       <c r="W98" s="37"/>
     </row>
-    <row r="99" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="29">
         <v>96</v>
       </c>
@@ -9838,7 +10011,7 @@
       <c r="V99" s="36"/>
       <c r="W99" s="37"/>
     </row>
-    <row r="100" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="29">
         <v>97</v>
       </c>
@@ -9873,7 +10046,7 @@
       <c r="V100" s="36"/>
       <c r="W100" s="37"/>
     </row>
-    <row r="101" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="29">
         <v>98</v>
       </c>
@@ -9908,7 +10081,7 @@
       <c r="V101" s="36"/>
       <c r="W101" s="37"/>
     </row>
-    <row r="102" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="29">
         <v>99</v>
       </c>
@@ -9943,7 +10116,7 @@
       <c r="V102" s="36"/>
       <c r="W102" s="37"/>
     </row>
-    <row r="103" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="29">
         <v>100</v>
       </c>
@@ -9978,7 +10151,7 @@
       <c r="V103" s="36"/>
       <c r="W103" s="37"/>
     </row>
-    <row r="104" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="29">
         <v>101</v>
       </c>
@@ -10013,7 +10186,7 @@
       <c r="V104" s="36"/>
       <c r="W104" s="37"/>
     </row>
-    <row r="105" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="29">
         <v>102</v>
       </c>
@@ -10048,7 +10221,7 @@
       <c r="V105" s="36"/>
       <c r="W105" s="37"/>
     </row>
-    <row r="106" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="29">
         <v>103</v>
       </c>
@@ -10083,7 +10256,7 @@
       <c r="V106" s="36"/>
       <c r="W106" s="37"/>
     </row>
-    <row r="107" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="29">
         <v>104</v>
       </c>
@@ -10118,7 +10291,7 @@
       <c r="V107" s="36"/>
       <c r="W107" s="37"/>
     </row>
-    <row r="108" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="29">
         <v>105</v>
       </c>
@@ -10153,7 +10326,7 @@
       <c r="V108" s="36"/>
       <c r="W108" s="37"/>
     </row>
-    <row r="109" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="29">
         <v>106</v>
       </c>
@@ -10188,7 +10361,7 @@
       <c r="V109" s="36"/>
       <c r="W109" s="37"/>
     </row>
-    <row r="110" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="29">
         <v>107</v>
       </c>
@@ -10223,7 +10396,7 @@
       <c r="V110" s="36"/>
       <c r="W110" s="37"/>
     </row>
-    <row r="111" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="29">
         <v>108</v>
       </c>
@@ -10258,7 +10431,7 @@
       <c r="V111" s="36"/>
       <c r="W111" s="37"/>
     </row>
-    <row r="112" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="29">
         <v>109</v>
       </c>
@@ -10293,7 +10466,7 @@
       <c r="V112" s="36"/>
       <c r="W112" s="37"/>
     </row>
-    <row r="113" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="29">
         <v>110</v>
       </c>
@@ -10328,7 +10501,7 @@
       <c r="V113" s="36"/>
       <c r="W113" s="37"/>
     </row>
-    <row r="114" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="29">
         <v>111</v>
       </c>
@@ -10363,7 +10536,7 @@
       <c r="V114" s="36"/>
       <c r="W114" s="37"/>
     </row>
-    <row r="115" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="29">
         <v>112</v>
       </c>
@@ -10398,7 +10571,7 @@
       <c r="V115" s="36"/>
       <c r="W115" s="37"/>
     </row>
-    <row r="116" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="29">
         <v>113</v>
       </c>
@@ -10433,7 +10606,7 @@
       <c r="V116" s="36"/>
       <c r="W116" s="37"/>
     </row>
-    <row r="117" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="29">
         <v>114</v>
       </c>
@@ -10468,7 +10641,7 @@
       <c r="V117" s="36"/>
       <c r="W117" s="37"/>
     </row>
-    <row r="118" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="29">
         <v>115</v>
       </c>
@@ -10503,7 +10676,7 @@
       <c r="V118" s="36"/>
       <c r="W118" s="37"/>
     </row>
-    <row r="119" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="29">
         <v>116</v>
       </c>
@@ -10538,7 +10711,7 @@
       <c r="V119" s="36"/>
       <c r="W119" s="37"/>
     </row>
-    <row r="120" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="29">
         <v>117</v>
       </c>
@@ -10573,7 +10746,7 @@
       <c r="V120" s="36"/>
       <c r="W120" s="37"/>
     </row>
-    <row r="121" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="29">
         <v>118</v>
       </c>
@@ -10608,7 +10781,7 @@
       <c r="V121" s="36"/>
       <c r="W121" s="37"/>
     </row>
-    <row r="122" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="29">
         <v>119</v>
       </c>
@@ -10643,7 +10816,7 @@
       <c r="V122" s="36"/>
       <c r="W122" s="37"/>
     </row>
-    <row r="123" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="29">
         <v>120</v>
       </c>
@@ -10678,7 +10851,7 @@
       <c r="V123" s="36"/>
       <c r="W123" s="37"/>
     </row>
-    <row r="124" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="29">
         <v>121</v>
       </c>
@@ -10758,8 +10931,12 @@
       <c r="P125" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q125" s="34"/>
-      <c r="R125" s="34"/>
+      <c r="Q125" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R125" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S125" s="69" t="s">
         <v>801</v>
       </c>
@@ -10817,8 +10994,12 @@
       <c r="P126" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q126" s="34"/>
-      <c r="R126" s="34"/>
+      <c r="Q126" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R126" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S126" s="69" t="s">
         <v>802</v>
       </c>
@@ -10876,8 +11057,12 @@
       <c r="P127" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q127" s="34"/>
-      <c r="R127" s="34"/>
+      <c r="Q127" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R127" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S127" s="69" t="s">
         <v>803</v>
       </c>
@@ -10935,8 +11120,12 @@
       <c r="P128" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q128" s="34"/>
-      <c r="R128" s="34"/>
+      <c r="Q128" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R128" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S128" s="69" t="s">
         <v>801</v>
       </c>
@@ -10994,8 +11183,12 @@
       <c r="P129" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q129" s="34"/>
-      <c r="R129" s="34"/>
+      <c r="Q129" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R129" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S129" s="69" t="s">
         <v>801</v>
       </c>
@@ -11053,8 +11246,12 @@
       <c r="P130" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q130" s="34"/>
-      <c r="R130" s="34"/>
+      <c r="Q130" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R130" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S130" s="69" t="s">
         <v>802</v>
       </c>
@@ -11112,8 +11309,12 @@
       <c r="P131" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q131" s="34"/>
-      <c r="R131" s="34"/>
+      <c r="Q131" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R131" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S131" s="69" t="s">
         <v>801</v>
       </c>
@@ -11171,8 +11372,12 @@
       <c r="P132" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q132" s="34"/>
-      <c r="R132" s="34"/>
+      <c r="Q132" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R132" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S132" s="69" t="s">
         <v>801</v>
       </c>
@@ -11230,8 +11435,12 @@
       <c r="P133" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q133" s="34"/>
-      <c r="R133" s="34"/>
+      <c r="Q133" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R133" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S133" s="69" t="s">
         <v>801</v>
       </c>
@@ -11289,8 +11498,12 @@
       <c r="P134" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q134" s="34"/>
-      <c r="R134" s="34"/>
+      <c r="Q134" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R134" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S134" s="69" t="s">
         <v>802</v>
       </c>
@@ -11348,8 +11561,12 @@
       <c r="P135" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q135" s="34"/>
-      <c r="R135" s="34"/>
+      <c r="Q135" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R135" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S135" s="69" t="s">
         <v>801</v>
       </c>
@@ -11407,8 +11624,12 @@
       <c r="P136" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q136" s="34"/>
-      <c r="R136" s="34"/>
+      <c r="Q136" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R136" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S136" s="69" t="s">
         <v>801</v>
       </c>
@@ -11466,8 +11687,12 @@
       <c r="P137" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q137" s="34"/>
-      <c r="R137" s="34"/>
+      <c r="Q137" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R137" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S137" s="69" t="s">
         <v>801</v>
       </c>
@@ -11525,8 +11750,12 @@
       <c r="P138" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q138" s="34"/>
-      <c r="R138" s="34"/>
+      <c r="Q138" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R138" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S138" s="69" t="s">
         <v>801</v>
       </c>
@@ -11584,8 +11813,12 @@
       <c r="P139" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q139" s="34"/>
-      <c r="R139" s="34"/>
+      <c r="Q139" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R139" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S139" s="69" t="s">
         <v>801</v>
       </c>
@@ -11643,8 +11876,12 @@
       <c r="P140" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q140" s="34"/>
-      <c r="R140" s="34"/>
+      <c r="Q140" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R140" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S140" s="69" t="s">
         <v>801</v>
       </c>
@@ -11702,8 +11939,12 @@
       <c r="P141" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q141" s="34"/>
-      <c r="R141" s="34"/>
+      <c r="Q141" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R141" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S141" s="69" t="s">
         <v>801</v>
       </c>
@@ -11761,8 +12002,12 @@
       <c r="P142" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q142" s="34"/>
-      <c r="R142" s="34"/>
+      <c r="Q142" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R142" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S142" s="69" t="s">
         <v>801</v>
       </c>
@@ -11820,8 +12065,12 @@
       <c r="P143" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q143" s="34"/>
-      <c r="R143" s="34"/>
+      <c r="Q143" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R143" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S143" s="69" t="s">
         <v>801</v>
       </c>
@@ -11879,8 +12128,12 @@
       <c r="P144" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q144" s="34"/>
-      <c r="R144" s="34"/>
+      <c r="Q144" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R144" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S144" s="69" t="s">
         <v>801</v>
       </c>
@@ -11938,8 +12191,12 @@
       <c r="P145" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q145" s="34"/>
-      <c r="R145" s="34"/>
+      <c r="Q145" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R145" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S145" s="69" t="s">
         <v>805</v>
       </c>
@@ -11997,8 +12254,12 @@
       <c r="P146" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q146" s="34"/>
-      <c r="R146" s="34"/>
+      <c r="Q146" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R146" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S146" s="69" t="s">
         <v>805</v>
       </c>
@@ -12056,8 +12317,12 @@
       <c r="P147" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q147" s="34"/>
-      <c r="R147" s="34"/>
+      <c r="Q147" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R147" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S147" s="69" t="s">
         <v>805</v>
       </c>
@@ -12115,8 +12380,12 @@
       <c r="P148" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="Q148" s="34"/>
-      <c r="R148" s="34"/>
+      <c r="Q148" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R148" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S148" s="69" t="s">
         <v>805</v>
       </c>
@@ -12174,8 +12443,12 @@
       <c r="P149" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q149" s="34"/>
-      <c r="R149" s="34"/>
+      <c r="Q149" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R149" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S149" s="69" t="s">
         <v>801</v>
       </c>
@@ -12478,8 +12751,12 @@
       <c r="P155" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q155" s="34"/>
-      <c r="R155" s="34"/>
+      <c r="Q155" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R155" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S155" s="34" t="s">
         <v>802</v>
       </c>
@@ -12537,8 +12814,12 @@
       <c r="P156" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q156" s="34"/>
-      <c r="R156" s="34"/>
+      <c r="Q156" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R156" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S156" s="34" t="s">
         <v>802</v>
       </c>
@@ -12596,8 +12877,12 @@
       <c r="P157" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q157" s="34"/>
-      <c r="R157" s="34"/>
+      <c r="Q157" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R157" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S157" s="34" t="s">
         <v>802</v>
       </c>
@@ -12655,8 +12940,12 @@
       <c r="P158" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q158" s="34"/>
-      <c r="R158" s="34"/>
+      <c r="Q158" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R158" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S158" s="34" t="s">
         <v>802</v>
       </c>
@@ -12714,8 +13003,12 @@
       <c r="P159" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q159" s="34"/>
-      <c r="R159" s="34"/>
+      <c r="Q159" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R159" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S159" s="34" t="s">
         <v>802</v>
       </c>
@@ -12773,8 +13066,12 @@
       <c r="P160" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q160" s="34"/>
-      <c r="R160" s="34"/>
+      <c r="Q160" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R160" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S160" s="34" t="s">
         <v>802</v>
       </c>
@@ -12832,8 +13129,12 @@
       <c r="P161" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q161" s="34"/>
-      <c r="R161" s="34"/>
+      <c r="Q161" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R161" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S161" s="34" t="s">
         <v>802</v>
       </c>
@@ -12891,8 +13192,12 @@
       <c r="P162" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q162" s="34"/>
-      <c r="R162" s="34"/>
+      <c r="Q162" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R162" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S162" s="34" t="s">
         <v>802</v>
       </c>
@@ -12950,8 +13255,12 @@
       <c r="P163" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q163" s="34"/>
-      <c r="R163" s="34"/>
+      <c r="Q163" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R163" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S163" s="34" t="s">
         <v>802</v>
       </c>
@@ -13009,8 +13318,12 @@
       <c r="P164" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q164" s="34"/>
-      <c r="R164" s="34"/>
+      <c r="Q164" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R164" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S164" s="34" t="s">
         <v>802</v>
       </c>
@@ -13068,8 +13381,12 @@
       <c r="P165" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q165" s="34"/>
-      <c r="R165" s="34"/>
+      <c r="Q165" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R165" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S165" s="34" t="s">
         <v>802</v>
       </c>
@@ -13127,8 +13444,12 @@
       <c r="P166" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q166" s="34"/>
-      <c r="R166" s="34"/>
+      <c r="Q166" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R166" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S166" s="34" t="s">
         <v>802</v>
       </c>
@@ -13186,8 +13507,12 @@
       <c r="P167" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q167" s="34"/>
-      <c r="R167" s="34"/>
+      <c r="Q167" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R167" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S167" s="34" t="s">
         <v>802</v>
       </c>
@@ -13245,8 +13570,12 @@
       <c r="P168" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q168" s="34"/>
-      <c r="R168" s="34"/>
+      <c r="Q168" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R168" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S168" s="34" t="s">
         <v>802</v>
       </c>
@@ -13304,8 +13633,12 @@
       <c r="P169" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q169" s="34"/>
-      <c r="R169" s="34"/>
+      <c r="Q169" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R169" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S169" s="34" t="s">
         <v>802</v>
       </c>
@@ -13363,8 +13696,12 @@
       <c r="P170" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q170" s="34"/>
-      <c r="R170" s="34"/>
+      <c r="Q170" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R170" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S170" s="34" t="s">
         <v>802</v>
       </c>
@@ -13422,8 +13759,12 @@
       <c r="P171" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q171" s="34"/>
-      <c r="R171" s="34"/>
+      <c r="Q171" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R171" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S171" s="34" t="s">
         <v>802</v>
       </c>
@@ -13481,8 +13822,12 @@
       <c r="P172" s="69" t="s">
         <v>305</v>
       </c>
-      <c r="Q172" s="34"/>
-      <c r="R172" s="34"/>
+      <c r="Q172" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="R172" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="S172" s="34" t="s">
         <v>802</v>
       </c>
@@ -13495,7 +13840,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="29">
         <v>174</v>
       </c>
@@ -13530,7 +13875,7 @@
       <c r="V173" s="36"/>
       <c r="W173" s="37"/>
     </row>
-    <row r="174" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="29">
         <v>175</v>
       </c>
@@ -13565,7 +13910,7 @@
       <c r="V174" s="36"/>
       <c r="W174" s="37"/>
     </row>
-    <row r="175" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="29">
         <v>176</v>
       </c>
@@ -13600,7 +13945,7 @@
       <c r="V175" s="36"/>
       <c r="W175" s="37"/>
     </row>
-    <row r="176" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="29">
         <v>177</v>
       </c>
@@ -13635,7 +13980,7 @@
       <c r="V176" s="36"/>
       <c r="W176" s="37"/>
     </row>
-    <row r="177" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="29">
         <v>178</v>
       </c>
@@ -13670,7 +14015,7 @@
       <c r="V177" s="36"/>
       <c r="W177" s="37"/>
     </row>
-    <row r="178" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="29">
         <v>179</v>
       </c>
@@ -13705,7 +14050,7 @@
       <c r="V178" s="36"/>
       <c r="W178" s="37"/>
     </row>
-    <row r="179" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="29">
         <v>180</v>
       </c>
@@ -13740,7 +14085,7 @@
       <c r="V179" s="36"/>
       <c r="W179" s="37"/>
     </row>
-    <row r="180" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="29">
         <v>181</v>
       </c>
@@ -13775,7 +14120,7 @@
       <c r="V180" s="36"/>
       <c r="W180" s="37"/>
     </row>
-    <row r="181" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="29">
         <v>182</v>
       </c>
@@ -13810,7 +14155,7 @@
       <c r="V181" s="36"/>
       <c r="W181" s="37"/>
     </row>
-    <row r="182" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="29">
         <v>183</v>
       </c>
@@ -13845,7 +14190,7 @@
       <c r="V182" s="36"/>
       <c r="W182" s="37"/>
     </row>
-    <row r="183" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="29">
         <v>184</v>
       </c>
@@ -13880,7 +14225,7 @@
       <c r="V183" s="36"/>
       <c r="W183" s="37"/>
     </row>
-    <row r="184" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="29">
         <v>185</v>
       </c>
@@ -13915,7 +14260,7 @@
       <c r="V184" s="36"/>
       <c r="W184" s="37"/>
     </row>
-    <row r="185" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="29">
         <v>186</v>
       </c>
@@ -13950,7 +14295,7 @@
       <c r="V185" s="36"/>
       <c r="W185" s="37"/>
     </row>
-    <row r="186" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="29">
         <v>187</v>
       </c>
@@ -13985,7 +14330,7 @@
       <c r="V186" s="36"/>
       <c r="W186" s="37"/>
     </row>
-    <row r="187" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="29">
         <v>188</v>
       </c>
@@ -14020,7 +14365,7 @@
       <c r="V187" s="36"/>
       <c r="W187" s="37"/>
     </row>
-    <row r="188" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="29">
         <v>189</v>
       </c>
@@ -14055,7 +14400,7 @@
       <c r="V188" s="36"/>
       <c r="W188" s="37"/>
     </row>
-    <row r="189" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="29">
         <v>190</v>
       </c>
@@ -14090,7 +14435,7 @@
       <c r="V189" s="36"/>
       <c r="W189" s="37"/>
     </row>
-    <row r="190" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="29">
         <v>191</v>
       </c>
@@ -14125,7 +14470,7 @@
       <c r="V190" s="36"/>
       <c r="W190" s="37"/>
     </row>
-    <row r="191" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="29">
         <v>368</v>
       </c>
@@ -14209,7 +14554,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="29">
         <v>371</v>
       </c>
@@ -14244,7 +14589,7 @@
       <c r="V193" s="36"/>
       <c r="W193" s="37"/>
     </row>
-    <row r="194" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A194" s="29">
         <v>372</v>
       </c>
@@ -14377,7 +14722,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="39">
         <v>376</v>
       </c>
@@ -14412,7 +14757,7 @@
       <c r="V197" s="46"/>
       <c r="W197" s="47"/>
     </row>
-    <row r="198" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="48">
         <v>417</v>
       </c>
@@ -14447,7 +14792,7 @@
       <c r="V198" s="55"/>
       <c r="W198" s="56"/>
     </row>
-    <row r="199" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="48">
         <v>418</v>
       </c>
@@ -14482,7 +14827,7 @@
       <c r="V199" s="55"/>
       <c r="W199" s="56"/>
     </row>
-    <row r="200" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="48">
         <v>419</v>
       </c>
@@ -14517,7 +14862,7 @@
       <c r="V200" s="55"/>
       <c r="W200" s="56"/>
     </row>
-    <row r="201" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="48">
         <v>423</v>
       </c>
@@ -14552,7 +14897,7 @@
       <c r="V201" s="55"/>
       <c r="W201" s="56"/>
     </row>
-    <row r="202" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="48">
         <v>424</v>
       </c>
@@ -14587,7 +14932,7 @@
       <c r="V202" s="55"/>
       <c r="W202" s="56"/>
     </row>
-    <row r="203" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="48">
         <v>425</v>
       </c>
@@ -14622,7 +14967,7 @@
       <c r="V203" s="55"/>
       <c r="W203" s="56"/>
     </row>
-    <row r="204" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="48">
         <v>426</v>
       </c>
@@ -14657,7 +15002,7 @@
       <c r="V204" s="55"/>
       <c r="W204" s="56"/>
     </row>
-    <row r="205" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A205" s="48">
         <v>427</v>
       </c>
@@ -14692,7 +15037,7 @@
       <c r="V205" s="55"/>
       <c r="W205" s="56"/>
     </row>
-    <row r="206" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="48">
         <v>428</v>
       </c>
@@ -14727,7 +15072,7 @@
       <c r="V206" s="55"/>
       <c r="W206" s="56"/>
     </row>
-    <row r="207" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A207" s="48">
         <v>429</v>
       </c>
@@ -14762,7 +15107,7 @@
       <c r="V207" s="55"/>
       <c r="W207" s="56"/>
     </row>
-    <row r="208" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A208" s="48">
         <v>430</v>
       </c>
@@ -14797,7 +15142,7 @@
       <c r="V208" s="55"/>
       <c r="W208" s="56"/>
     </row>
-    <row r="209" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="48">
         <v>431</v>
       </c>
@@ -14832,7 +15177,7 @@
       <c r="V209" s="55"/>
       <c r="W209" s="56"/>
     </row>
-    <row r="210" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A210" s="48">
         <v>432</v>
       </c>
@@ -14867,7 +15212,7 @@
       <c r="V210" s="55"/>
       <c r="W210" s="56"/>
     </row>
-    <row r="211" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A211" s="48">
         <v>433</v>
       </c>
@@ -14902,7 +15247,7 @@
       <c r="V211" s="55"/>
       <c r="W211" s="56"/>
     </row>
-    <row r="212" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A212" s="48">
         <v>434</v>
       </c>
@@ -14937,7 +15282,7 @@
       <c r="V212" s="55"/>
       <c r="W212" s="56"/>
     </row>
-    <row r="213" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A213" s="48">
         <v>435</v>
       </c>
@@ -14972,7 +15317,7 @@
       <c r="V213" s="55"/>
       <c r="W213" s="56"/>
     </row>
-    <row r="214" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A214" s="48">
         <v>436</v>
       </c>
@@ -15007,7 +15352,7 @@
       <c r="V214" s="55"/>
       <c r="W214" s="56"/>
     </row>
-    <row r="215" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A215" s="48">
         <v>437</v>
       </c>
@@ -15042,7 +15387,7 @@
       <c r="V215" s="55"/>
       <c r="W215" s="56"/>
     </row>
-    <row r="216" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A216" s="48">
         <v>438</v>
       </c>
@@ -15077,7 +15422,7 @@
       <c r="V216" s="55"/>
       <c r="W216" s="56"/>
     </row>
-    <row r="217" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A217" s="48">
         <v>439</v>
       </c>
@@ -15112,7 +15457,7 @@
       <c r="V217" s="55"/>
       <c r="W217" s="56"/>
     </row>
-    <row r="218" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A218" s="48">
         <v>440</v>
       </c>
@@ -15147,7 +15492,7 @@
       <c r="V218" s="55"/>
       <c r="W218" s="56"/>
     </row>
-    <row r="219" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A219" s="48">
         <v>441</v>
       </c>
@@ -15182,7 +15527,7 @@
       <c r="V219" s="55"/>
       <c r="W219" s="56"/>
     </row>
-    <row r="220" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A220" s="57">
         <v>442</v>
       </c>
@@ -15217,7 +15562,7 @@
       <c r="V220" s="64"/>
       <c r="W220" s="65"/>
     </row>
-    <row r="221" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A221" s="48">
         <v>443</v>
       </c>
@@ -15252,7 +15597,7 @@
       <c r="V221" s="55"/>
       <c r="W221" s="56"/>
     </row>
-    <row r="222" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A222" s="48">
         <v>444</v>
       </c>
@@ -15287,7 +15632,7 @@
       <c r="V222" s="55"/>
       <c r="W222" s="56"/>
     </row>
-    <row r="223" spans="1:23" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:23" ht="40.799999999999997" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A223" s="48">
         <v>445</v>
       </c>
@@ -20012,7 +20357,16 @@
       <c r="W809" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W225" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W225" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="LDO"/>
+        <filter val="RAD"/>
+        <filter val="RSA"/>
+        <filter val="VPS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -20033,7 +20387,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J55:J65 P31 J31 M31:N31 Q34:R34 J197:J223 P39 J39 M39:N39 Q42:R42 P47 M197:N223 J47 J10:J14 J19:J26 J36:J37 J44:J45 J52:J53 J97:J124 J173:J191 J193:J194 M19:N26 M36:N37 M47:N47 M10:N14 M44:N45 M52:N53 M55:N65 M97:N124 M173:N191 M193:N194 Q10:R32 P10:P14 P19:P26 Q36:R40 P36:P37 Q44:R48 P44:P45 Q50:R225 P52:P53 P55:P65 P97:P124 P173:P191 P193:P194 P197:P223</xm:sqref>
+          <xm:sqref>J55:J65 P31 J31 M31:N31 P197:P223 J197:J223 P39 J39 M39:N39 Q34:R40 P47 M197:N223 J47 J10:J14 J19:J26 J36:J37 J44:J45 J52:J53 J97:J124 J173:J191 J193:J194 M19:N26 M36:N37 M47:N47 M10:N14 M44:N45 M52:N53 M55:N65 M97:N124 M173:N191 M193:N194 Q10:R32 P10:P14 P19:P26 P36:P37 P44:P45 Q42:R48 P52:P53 P55:P65 P97:P124 P173:P191 P193:P194 Q50:R225</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -22292,27 +22646,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -22570,10 +22903,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22596,20 +22961,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>